<commit_message>
major refactor add write_to_file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\report_card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\report_card\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5895" tabRatio="412" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5897" tabRatio="412" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="машинисты" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="186">
   <si>
     <t>Код</t>
   </si>
@@ -583,10 +583,7 @@
     <t>/8</t>
   </si>
   <si>
-    <t>/8 20/</t>
-  </si>
-  <si>
-    <t>20=</t>
+    <t xml:space="preserve"> 20/</t>
   </si>
 </sst>
 </file>
@@ -1507,31 +1504,31 @@
       <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="7.6328125" customWidth="1"/>
     <col min="4" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
     <col min="16" max="16" width="6" customWidth="1"/>
-    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="5.5" customWidth="1"/>
-    <col min="20" max="20" width="5.1640625" customWidth="1"/>
-    <col min="21" max="21" width="4.1640625" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" customWidth="1"/>
-    <col min="23" max="23" width="4.5" customWidth="1"/>
-    <col min="24" max="24" width="5.1640625" customWidth="1"/>
+    <col min="19" max="19" width="5.453125" customWidth="1"/>
+    <col min="20" max="20" width="5.1796875" customWidth="1"/>
+    <col min="21" max="21" width="4.1796875" customWidth="1"/>
+    <col min="22" max="22" width="5.36328125" customWidth="1"/>
+    <col min="23" max="23" width="4.453125" customWidth="1"/>
+    <col min="24" max="24" width="5.1796875" customWidth="1"/>
     <col min="25" max="25" width="4" customWidth="1"/>
     <col min="26" max="26" width="5" customWidth="1"/>
-    <col min="27" max="27" width="6.83203125" customWidth="1"/>
+    <col min="27" max="27" width="6.81640625" customWidth="1"/>
     <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="6.6640625" customWidth="1"/>
-    <col min="30" max="30" width="7.33203125" customWidth="1"/>
+    <col min="29" max="29" width="6.6328125" customWidth="1"/>
+    <col min="30" max="30" width="7.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:40" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
         <v>1</v>
       </c>
@@ -1567,7 +1564,7 @@
       <c r="AE1" s="9"/>
       <c r="AF1" s="9"/>
     </row>
-    <row r="2" spans="1:40" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:40" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="101" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1598,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:40" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:40" s="6" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
         <v>101</v>
       </c>
@@ -1637,7 +1634,7 @@
       <c r="AE3" s="10"/>
       <c r="AF3" s="10"/>
     </row>
-    <row r="4" spans="1:40" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:40" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>3</v>
       </c>
@@ -1666,7 +1663,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:40" s="6" customFormat="1" ht="7.9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:40" s="6" customFormat="1" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="15"/>
       <c r="R5" s="70" t="s">
         <v>4</v>
@@ -1692,7 +1689,7 @@
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
     </row>
-    <row r="6" spans="1:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q6" s="15"/>
       <c r="R6" s="72"/>
       <c r="S6" s="72"/>
@@ -1714,7 +1711,7 @@
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
     </row>
-    <row r="7" spans="1:40" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:40" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K7" s="94" t="s">
         <v>9</v>
       </c>
@@ -1748,7 +1745,7 @@
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
     </row>
-    <row r="8" spans="1:40" s="14" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" s="14" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J8" s="94" t="s">
         <v>83</v>
       </c>
@@ -1761,7 +1758,7 @@
       <c r="Q8" s="94"/>
       <c r="R8" s="94"/>
     </row>
-    <row r="9" spans="1:40" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104" t="s">
         <v>45</v>
       </c>
@@ -1806,7 +1803,7 @@
       </c>
       <c r="AC9" s="96"/>
     </row>
-    <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="105"/>
       <c r="B10" s="107"/>
       <c r="C10" s="28" t="s">
@@ -1885,7 +1882,7 @@
       <c r="AB10" s="96"/>
       <c r="AC10" s="96"/>
     </row>
-    <row r="11" spans="1:40" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="105"/>
       <c r="B11" s="107"/>
       <c r="C11" s="66" t="s">
@@ -1955,7 +1952,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>11</v>
       </c>
@@ -2017,7 +2014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="77">
         <v>1</v>
       </c>
@@ -2103,7 +2100,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="80"/>
       <c r="C14" s="33" t="s">
@@ -2167,7 +2164,7 @@
       <c r="AC14" s="86"/>
       <c r="AD14" s="89"/>
     </row>
-    <row r="15" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="77">
         <v>2</v>
       </c>
@@ -2249,7 +2246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="78"/>
       <c r="C16" s="33" t="s">
@@ -2313,7 +2310,7 @@
       <c r="AC16" s="89"/>
       <c r="AD16" s="89"/>
     </row>
-    <row r="17" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="77">
         <v>3</v>
       </c>
@@ -2395,7 +2392,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
       <c r="B18" s="78"/>
       <c r="C18" s="33" t="s">
@@ -2459,7 +2456,7 @@
       <c r="AC18" s="87"/>
       <c r="AD18" s="87"/>
     </row>
-    <row r="19" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="77">
         <v>4</v>
       </c>
@@ -2541,7 +2538,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
       <c r="B20" s="80"/>
       <c r="C20" s="41" t="s">
@@ -2605,7 +2602,7 @@
       <c r="AC20" s="87"/>
       <c r="AD20" s="89"/>
     </row>
-    <row r="21" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77">
         <v>5</v>
       </c>
@@ -2689,7 +2686,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="77"/>
       <c r="B22" s="78"/>
       <c r="C22" s="33" t="s">
@@ -2753,7 +2750,7 @@
       <c r="AC22" s="86"/>
       <c r="AD22" s="89"/>
     </row>
-    <row r="23" spans="1:30" s="27" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="27" customFormat="1" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="90">
         <v>6</v>
       </c>
@@ -2835,7 +2832,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="27" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="27" customFormat="1" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="90"/>
       <c r="B24" s="78"/>
       <c r="C24" s="58" t="s">
@@ -2899,7 +2896,7 @@
       <c r="AC24" s="87"/>
       <c r="AD24" s="87"/>
     </row>
-    <row r="25" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="77">
         <v>7</v>
       </c>
@@ -2983,7 +2980,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="77"/>
       <c r="B26" s="78"/>
       <c r="C26" s="33" t="s">
@@ -3047,7 +3044,7 @@
       <c r="AC26" s="87"/>
       <c r="AD26" s="87"/>
     </row>
-    <row r="27" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="77">
         <v>8</v>
       </c>
@@ -3131,7 +3128,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="77"/>
       <c r="B28" s="78"/>
       <c r="C28" s="36" t="s">
@@ -3195,7 +3192,7 @@
       <c r="AC28" s="87"/>
       <c r="AD28" s="87"/>
     </row>
-    <row r="29" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="77">
         <v>9</v>
       </c>
@@ -3279,7 +3276,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77"/>
       <c r="B30" s="78"/>
       <c r="C30" s="33" t="s">
@@ -3343,7 +3340,7 @@
       <c r="AC30" s="87"/>
       <c r="AD30" s="85"/>
     </row>
-    <row r="31" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="77">
         <v>10</v>
       </c>
@@ -3425,7 +3422,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="77"/>
       <c r="B32" s="78"/>
       <c r="C32" s="50" t="s">
@@ -3489,7 +3486,7 @@
       <c r="AC32" s="87"/>
       <c r="AD32" s="87"/>
     </row>
-    <row r="33" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="77">
         <v>11</v>
       </c>
@@ -3573,7 +3570,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="77"/>
       <c r="B34" s="78"/>
       <c r="C34" s="36" t="s">
@@ -3637,7 +3634,7 @@
       <c r="AC34" s="87"/>
       <c r="AD34" s="89"/>
     </row>
-    <row r="35" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="77">
         <v>12</v>
       </c>
@@ -3713,7 +3710,7 @@
       <c r="AC35" s="87"/>
       <c r="AD35" s="87"/>
     </row>
-    <row r="36" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="77"/>
       <c r="B36" s="78"/>
       <c r="C36" s="58" t="s">
@@ -3777,7 +3774,7 @@
       <c r="AC36" s="87"/>
       <c r="AD36" s="87"/>
     </row>
-    <row r="37" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="77">
         <v>13</v>
       </c>
@@ -3851,7 +3848,7 @@
       <c r="AC37" s="87"/>
       <c r="AD37" s="87"/>
     </row>
-    <row r="38" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="77"/>
       <c r="B38" s="78"/>
       <c r="C38" s="33" t="s">
@@ -3915,7 +3912,7 @@
       <c r="AC38" s="87"/>
       <c r="AD38" s="87"/>
     </row>
-    <row r="39" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77">
         <v>14</v>
       </c>
@@ -3989,7 +3986,7 @@
       <c r="AC39" s="87"/>
       <c r="AD39" s="87"/>
     </row>
-    <row r="40" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="77"/>
       <c r="B40" s="78"/>
       <c r="C40" s="33" t="s">
@@ -4053,7 +4050,7 @@
       <c r="AC40" s="87"/>
       <c r="AD40" s="87"/>
     </row>
-    <row r="41" spans="1:30" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="17"/>
       <c r="C41" s="18"/>
@@ -4085,7 +4082,7 @@
       <c r="AC41" s="19"/>
       <c r="AD41" s="19"/>
     </row>
-    <row r="42" spans="1:30" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
         <v>102</v>
       </c>
@@ -4123,7 +4120,7 @@
       <c r="AC42" s="19"/>
       <c r="AD42" s="19"/>
     </row>
-    <row r="43" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="74"/>
       <c r="B43" s="74"/>
       <c r="C43" s="74"/>
@@ -4159,7 +4156,7 @@
       <c r="AC43" s="19"/>
       <c r="AD43" s="19"/>
     </row>
-    <row r="44" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
         <v>44</v>
       </c>
@@ -4197,7 +4194,7 @@
       <c r="AC44" s="6"/>
       <c r="AD44" s="6"/>
     </row>
-    <row r="45" spans="1:30" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" ht="9.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="74"/>
       <c r="B45" s="74"/>
       <c r="C45" s="74"/>
@@ -4233,7 +4230,7 @@
       <c r="AC45" s="6"/>
       <c r="AD45" s="6"/>
     </row>
-    <row r="46" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
         <v>59</v>
       </c>
@@ -4271,7 +4268,7 @@
       <c r="AC46" s="6"/>
       <c r="AD46" s="6"/>
     </row>
-    <row r="47" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="74"/>
       <c r="B47" s="74"/>
       <c r="C47" s="74"/>
@@ -4307,7 +4304,7 @@
       <c r="AC47" s="6"/>
       <c r="AD47" s="6"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -4339,7 +4336,7 @@
       <c r="AC48" s="6"/>
       <c r="AD48" s="6"/>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -4371,7 +4368,7 @@
       <c r="AC49" s="6"/>
       <c r="AD49" s="6"/>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -4403,7 +4400,7 @@
       <c r="AC50" s="6"/>
       <c r="AD50" s="6"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -4435,7 +4432,7 @@
       <c r="AC51" s="6"/>
       <c r="AD51" s="6"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -4727,31 +4724,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13:S14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10:AB11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="16" width="6.5" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" customWidth="1"/>
-    <col min="19" max="19" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="16" width="6.453125" customWidth="1"/>
+    <col min="17" max="17" width="7.81640625" customWidth="1"/>
+    <col min="18" max="18" width="8.6328125" customWidth="1"/>
+    <col min="19" max="19" width="4.6328125" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="3.5" customWidth="1"/>
-    <col min="22" max="22" width="5.33203125" customWidth="1"/>
-    <col min="23" max="23" width="5.5" customWidth="1"/>
-    <col min="24" max="25" width="4.1640625" customWidth="1"/>
-    <col min="26" max="27" width="4.83203125" customWidth="1"/>
-    <col min="28" max="28" width="4.5" customWidth="1"/>
+    <col min="21" max="21" width="3.453125" customWidth="1"/>
+    <col min="22" max="22" width="5.36328125" customWidth="1"/>
+    <col min="23" max="23" width="5.453125" customWidth="1"/>
+    <col min="24" max="25" width="4.1796875" customWidth="1"/>
+    <col min="26" max="27" width="4.81640625" customWidth="1"/>
+    <col min="28" max="28" width="4.453125" customWidth="1"/>
     <col min="29" max="30" width="6" customWidth="1"/>
-    <col min="31" max="31" width="5.5" customWidth="1"/>
+    <col min="31" max="31" width="5.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:41" s="6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
         <v>1</v>
       </c>
@@ -4788,7 +4785,7 @@
       <c r="AF1" s="9"/>
       <c r="AG1" s="9"/>
     </row>
-    <row r="2" spans="1:41" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:41" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="101" t="s">
         <v>2</v>
       </c>
@@ -4823,7 +4820,7 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
     </row>
-    <row r="3" spans="1:41" s="6" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:41" s="6" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
         <v>101</v>
       </c>
@@ -4860,7 +4857,7 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
     </row>
-    <row r="4" spans="1:41" s="6" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" s="6" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>3</v>
       </c>
@@ -4889,7 +4886,7 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
     </row>
-    <row r="5" spans="1:41" s="6" customFormat="1" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:41" s="6" customFormat="1" ht="8.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="15"/>
       <c r="R5" s="70" t="s">
         <v>4</v>
@@ -4916,7 +4913,7 @@
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
     </row>
-    <row r="6" spans="1:41" s="6" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" s="6" customFormat="1" ht="9.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q6" s="15"/>
       <c r="R6" s="72"/>
       <c r="S6" s="72"/>
@@ -4939,7 +4936,7 @@
       <c r="AF6" s="7"/>
       <c r="AG6" s="7"/>
     </row>
-    <row r="7" spans="1:41" s="6" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:41" s="6" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K7" s="94" t="s">
         <v>9</v>
       </c>
@@ -4974,7 +4971,7 @@
       <c r="AF7" s="8"/>
       <c r="AG7" s="8"/>
     </row>
-    <row r="8" spans="1:41" s="14" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" s="14" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J8" s="94" t="s">
         <v>83</v>
       </c>
@@ -4987,7 +4984,7 @@
       <c r="Q8" s="94"/>
       <c r="R8" s="94"/>
     </row>
-    <row r="9" spans="1:41" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="122" t="s">
         <v>45</v>
       </c>
@@ -5033,7 +5030,7 @@
       </c>
       <c r="AD9" s="96"/>
     </row>
-    <row r="10" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="123"/>
       <c r="B10" s="123"/>
       <c r="C10" s="28" t="s">
@@ -5115,7 +5112,7 @@
       <c r="AC10" s="96"/>
       <c r="AD10" s="96"/>
     </row>
-    <row r="11" spans="1:41" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="123"/>
       <c r="B11" s="123"/>
       <c r="C11" s="61" t="s">
@@ -5186,7 +5183,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:41" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>11</v>
       </c>
@@ -5249,7 +5246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="77">
         <v>1</v>
       </c>
@@ -5305,7 +5302,7 @@
         <v>40</v>
       </c>
       <c r="S13" s="88" t="s">
-        <v>186</v>
+        <v>30</v>
       </c>
       <c r="T13" s="88" t="s">
         <v>158</v>
@@ -5334,7 +5331,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="78"/>
       <c r="C14" s="33" t="s">
@@ -5399,7 +5396,7 @@
       <c r="AD14" s="87"/>
       <c r="AE14" s="87"/>
     </row>
-    <row r="15" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="77">
         <v>2</v>
       </c>
@@ -5482,7 +5479,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="78"/>
       <c r="C16" s="38" t="s">
@@ -5547,7 +5544,7 @@
       <c r="AD16" s="87"/>
       <c r="AE16" s="128"/>
     </row>
-    <row r="17" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="77">
         <v>3</v>
       </c>
@@ -5564,7 +5561,7 @@
         <v>182</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>39</v>
@@ -5588,7 +5585,7 @@
         <v>182</v>
       </c>
       <c r="N17" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="O17" s="33" t="s">
         <v>39</v>
@@ -5632,7 +5629,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
       <c r="B18" s="78"/>
       <c r="C18" s="33" t="s">
@@ -5648,7 +5645,7 @@
         <v>182</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>39</v>
@@ -5697,7 +5694,7 @@
       <c r="AD18" s="87"/>
       <c r="AE18" s="87"/>
     </row>
-    <row r="19" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="77">
         <v>4</v>
       </c>
@@ -5708,7 +5705,7 @@
         <v>133</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>39</v>
@@ -5732,7 +5729,7 @@
         <v>182</v>
       </c>
       <c r="L19" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="M19" s="33" t="s">
         <v>39</v>
@@ -5782,7 +5779,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
       <c r="B20" s="78"/>
       <c r="C20" s="36" t="s">
@@ -5792,7 +5789,7 @@
         <v>182</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="F20" s="33" t="s">
         <v>39</v>
@@ -5816,7 +5813,7 @@
         <v>182</v>
       </c>
       <c r="M20" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="N20" s="33" t="s">
         <v>39</v>
@@ -5847,7 +5844,7 @@
       <c r="AD20" s="87"/>
       <c r="AE20" s="87"/>
     </row>
-    <row r="21" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77">
         <v>5</v>
       </c>
@@ -5858,7 +5855,7 @@
         <v>133</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>39</v>
@@ -5882,7 +5879,7 @@
         <v>182</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="M21" s="33" t="s">
         <v>39</v>
@@ -5932,7 +5929,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="77"/>
       <c r="B22" s="78"/>
       <c r="C22" s="36" t="s">
@@ -5942,7 +5939,7 @@
         <v>182</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="F22" s="33" t="s">
         <v>39</v>
@@ -5966,7 +5963,7 @@
         <v>182</v>
       </c>
       <c r="M22" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="N22" s="33" t="s">
         <v>39</v>
@@ -5997,7 +5994,7 @@
       <c r="AD22" s="87"/>
       <c r="AE22" s="87"/>
     </row>
-    <row r="23" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="77">
         <v>6</v>
       </c>
@@ -6014,7 +6011,7 @@
         <v>182</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="G23" s="33" t="s">
         <v>39</v>
@@ -6038,7 +6035,7 @@
         <v>182</v>
       </c>
       <c r="N23" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="O23" s="33" t="s">
         <v>39</v>
@@ -6082,7 +6079,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="77"/>
       <c r="B24" s="78"/>
       <c r="C24" s="33" t="s">
@@ -6098,7 +6095,7 @@
         <v>182</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>39</v>
@@ -6122,7 +6119,7 @@
         <v>182</v>
       </c>
       <c r="O24" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="P24" s="33" t="s">
         <v>39</v>
@@ -6147,7 +6144,7 @@
       <c r="AD24" s="87"/>
       <c r="AE24" s="87"/>
     </row>
-    <row r="25" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="77">
         <v>7</v>
       </c>
@@ -6170,7 +6167,7 @@
         <v>182</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="I25" s="33" t="s">
         <v>39</v>
@@ -6194,7 +6191,7 @@
         <v>182</v>
       </c>
       <c r="P25" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="Q25" s="33" t="s">
         <v>39</v>
@@ -6232,7 +6229,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="77"/>
       <c r="B26" s="78"/>
       <c r="C26" s="33" t="s">
@@ -6254,7 +6251,7 @@
         <v>182</v>
       </c>
       <c r="I26" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>39</v>
@@ -6278,7 +6275,7 @@
         <v>182</v>
       </c>
       <c r="Q26" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="R26" s="33" t="s">
         <v>39</v>
@@ -6297,7 +6294,7 @@
       <c r="AD26" s="87"/>
       <c r="AE26" s="87"/>
     </row>
-    <row r="27" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="77">
         <v>8</v>
       </c>
@@ -6382,7 +6379,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="77"/>
       <c r="B28" s="78"/>
       <c r="C28" s="33" t="s">
@@ -6416,13 +6413,13 @@
         <v>18</v>
       </c>
       <c r="M28" s="33" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="N28" s="33" t="s">
         <v>182</v>
       </c>
       <c r="O28" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="P28" s="33" t="s">
         <v>39</v>
@@ -6447,7 +6444,7 @@
       <c r="AD28" s="87"/>
       <c r="AE28" s="87"/>
     </row>
-    <row r="29" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="77">
         <v>9</v>
       </c>
@@ -6476,7 +6473,7 @@
         <v>182</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="K29" s="33" t="s">
         <v>39</v>
@@ -6534,7 +6531,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77"/>
       <c r="B30" s="78"/>
       <c r="C30" s="33" t="s">
@@ -6599,7 +6596,7 @@
       <c r="AD30" s="87"/>
       <c r="AE30" s="87"/>
     </row>
-    <row r="31" spans="1:31" s="27" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" s="27" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="90">
         <v>10</v>
       </c>
@@ -6684,7 +6681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:31" s="27" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" s="27" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="90"/>
       <c r="B32" s="78"/>
       <c r="C32" s="33" t="s">
@@ -6749,7 +6746,7 @@
       <c r="AD32" s="89"/>
       <c r="AE32" s="87"/>
     </row>
-    <row r="33" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="77">
         <v>11</v>
       </c>
@@ -6778,7 +6775,7 @@
         <v>182</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="K33" s="33" t="s">
         <v>39</v>
@@ -6832,7 +6829,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="77"/>
       <c r="B34" s="78"/>
       <c r="C34" s="38" t="s">
@@ -6860,7 +6857,7 @@
         <v>182</v>
       </c>
       <c r="K34" s="38" t="s">
-        <v>18</v>
+        <v>184</v>
       </c>
       <c r="L34" s="33" t="s">
         <v>39</v>
@@ -6885,7 +6882,7 @@
       <c r="AD34" s="87"/>
       <c r="AE34" s="87"/>
     </row>
-    <row r="35" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="77">
         <v>12</v>
       </c>
@@ -6962,7 +6959,7 @@
       <c r="AD35" s="87"/>
       <c r="AE35" s="87"/>
     </row>
-    <row r="36" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="77"/>
       <c r="B36" s="124"/>
       <c r="C36" s="33" t="s">
@@ -7027,7 +7024,7 @@
       <c r="AD36" s="87"/>
       <c r="AE36" s="87"/>
     </row>
-    <row r="37" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="77">
         <v>13</v>
       </c>
@@ -7102,7 +7099,7 @@
       <c r="AD37" s="87"/>
       <c r="AE37" s="87"/>
     </row>
-    <row r="38" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="77"/>
       <c r="B38" s="124"/>
       <c r="C38" s="33" t="s">
@@ -7167,7 +7164,7 @@
       <c r="AD38" s="87"/>
       <c r="AE38" s="87"/>
     </row>
-    <row r="39" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77">
         <v>14</v>
       </c>
@@ -7242,7 +7239,7 @@
       <c r="AD39" s="87"/>
       <c r="AE39" s="87"/>
     </row>
-    <row r="40" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="77"/>
       <c r="B40" s="124"/>
       <c r="C40" s="33" t="s">
@@ -7307,7 +7304,7 @@
       <c r="AD40" s="87"/>
       <c r="AE40" s="87"/>
     </row>
-    <row r="41" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="77">
         <v>15</v>
       </c>
@@ -7384,7 +7381,7 @@
       <c r="AD41" s="87"/>
       <c r="AE41" s="87"/>
     </row>
-    <row r="42" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="77"/>
       <c r="B42" s="124"/>
       <c r="C42" s="33" t="s">
@@ -7449,7 +7446,7 @@
       <c r="AD42" s="87"/>
       <c r="AE42" s="87"/>
     </row>
-    <row r="43" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="77">
         <v>16</v>
       </c>
@@ -7524,7 +7521,7 @@
       <c r="AD43" s="87"/>
       <c r="AE43" s="87"/>
     </row>
-    <row r="44" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:31" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="77"/>
       <c r="B44" s="124"/>
       <c r="C44" s="33" t="s">
@@ -7589,7 +7586,7 @@
       <c r="AD44" s="87"/>
       <c r="AE44" s="87"/>
     </row>
-    <row r="45" spans="1:31" ht="5.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:31" ht="5.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="17"/>
       <c r="C45" s="18"/>
@@ -7622,7 +7619,7 @@
       <c r="AD45" s="19"/>
       <c r="AE45" s="19"/>
     </row>
-    <row r="46" spans="1:31" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:31" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
         <v>102</v>
       </c>
@@ -7661,7 +7658,7 @@
       <c r="AD46" s="19"/>
       <c r="AE46" s="19"/>
     </row>
-    <row r="47" spans="1:31" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:31" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="74"/>
       <c r="B47" s="74"/>
       <c r="C47" s="74"/>
@@ -7698,7 +7695,7 @@
       <c r="AD47" s="19"/>
       <c r="AE47" s="19"/>
     </row>
-    <row r="48" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
         <v>44</v>
       </c>
@@ -7737,7 +7734,7 @@
       <c r="AD48" s="6"/>
       <c r="AE48" s="6"/>
     </row>
-    <row r="49" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="74"/>
       <c r="B49" s="74"/>
       <c r="C49" s="74"/>
@@ -7774,7 +7771,7 @@
       <c r="AD49" s="6"/>
       <c r="AE49" s="6"/>
     </row>
-    <row r="50" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
         <v>59</v>
       </c>
@@ -7813,7 +7810,7 @@
       <c r="AD50" s="6"/>
       <c r="AE50" s="6"/>
     </row>
-    <row r="51" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="74"/>
       <c r="B51" s="74"/>
       <c r="C51" s="74"/>
@@ -7850,7 +7847,7 @@
       <c r="AD51" s="6"/>
       <c r="AE51" s="6"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -7883,7 +7880,7 @@
       <c r="AD52" s="6"/>
       <c r="AE52" s="6"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -7916,7 +7913,7 @@
       <c r="AD53" s="6"/>
       <c r="AE53" s="6"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -7949,7 +7946,7 @@
       <c r="AD54" s="6"/>
       <c r="AE54" s="6"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -7982,7 +7979,7 @@
       <c r="AD55" s="6"/>
       <c r="AE55" s="6"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -8323,12 +8320,12 @@
       <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="132.5" customWidth="1"/>
+    <col min="1" max="1" width="132.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>64</v>
       </c>
@@ -8336,7 +8333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>65</v>
       </c>
@@ -8344,7 +8341,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>66</v>
       </c>
@@ -8352,7 +8349,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>68</v>
       </c>
@@ -8360,7 +8357,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>69</v>
       </c>
@@ -8368,7 +8365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>70</v>
       </c>
@@ -8376,7 +8373,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>71</v>
       </c>
@@ -8384,7 +8381,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>72</v>
       </c>
@@ -8392,7 +8389,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>73</v>
       </c>
@@ -8400,7 +8397,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>74</v>
       </c>
@@ -8408,7 +8405,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>76</v>
       </c>
@@ -8416,7 +8413,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>78</v>
       </c>
@@ -8424,7 +8421,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>80</v>
       </c>
@@ -8432,7 +8429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>84</v>
       </c>
@@ -8440,7 +8437,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="12.9" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
trying classes 3 iteration add normalize method
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="179">
   <si>
     <t>ГОСУДАРСТВЕННОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ НЕНЕЦКОГО АВТОНОМНОГО ОКРУГА "НАРЬЯН-МАРСКАЯ ЭЛЕКТРОСТАНЦИЯ"</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>/8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 20/</t>
   </si>
   <si>
     <t>Баранов Р.А. Эл.монтер ЩУ ГТУ</t>
@@ -4648,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5290,18 +5287,16 @@
       <c r="N14" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="O14" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="P14" s="17" t="s">
-        <v>127</v>
+      <c r="O14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="R14" s="17" t="s">
-        <v>59</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="R14" s="17"/>
       <c r="S14" s="48"/>
       <c r="T14" s="48"/>
       <c r="U14" s="48"/>
@@ -5321,7 +5316,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>59</v>
@@ -5366,7 +5361,7 @@
         <v>60</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R15" s="39" t="s">
         <v>62</v>
@@ -5450,7 +5445,7 @@
         <v>60</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S16" s="48"/>
       <c r="T16" s="48"/>
@@ -5471,7 +5466,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="39" t="s">
         <v>59</v>
@@ -5544,13 +5539,13 @@
       <c r="AA17" s="49"/>
       <c r="AB17" s="49"/>
       <c r="AC17" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD17" s="49" t="s">
         <v>87</v>
       </c>
       <c r="AE17" s="49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -5578,31 +5573,31 @@
         <v>59</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S18" s="48"/>
       <c r="T18" s="48"/>
@@ -5623,7 +5618,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>91</v>
@@ -5700,7 +5695,7 @@
         <v>49</v>
       </c>
       <c r="AE19" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -5773,7 +5768,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>91</v>
@@ -5850,7 +5845,7 @@
         <v>49</v>
       </c>
       <c r="AE21" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -5923,7 +5918,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C23" s="39" t="s">
         <v>59</v>
@@ -5996,13 +5991,13 @@
       <c r="AA23" s="49"/>
       <c r="AB23" s="49"/>
       <c r="AC23" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD23" s="49" t="s">
         <v>53</v>
       </c>
       <c r="AE23" s="49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -6054,7 +6049,7 @@
         <v>59</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S24" s="48"/>
       <c r="T24" s="48"/>
@@ -6075,7 +6070,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>58</v>
@@ -6225,7 +6220,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>59</v>
@@ -6377,7 +6372,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>59</v>
@@ -6456,7 +6451,7 @@
         <v>98</v>
       </c>
       <c r="AE29" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -6484,31 +6479,31 @@
         <v>67</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S30" s="48"/>
       <c r="T30" s="48"/>
@@ -6529,7 +6524,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>59</v>
@@ -6658,7 +6653,7 @@
         <v>60</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S32" s="48"/>
       <c r="T32" s="48"/>
@@ -6679,7 +6674,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>59</v>
@@ -6724,7 +6719,7 @@
         <v>60</v>
       </c>
       <c r="Q33" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R33" s="39" t="s">
         <v>62</v>
@@ -6748,7 +6743,7 @@
       <c r="AA33" s="49"/>
       <c r="AB33" s="49"/>
       <c r="AC33" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AD33" s="49" t="s">
         <v>64</v>
@@ -6815,25 +6810,25 @@
         <v>12</v>
       </c>
       <c r="B35" s="101" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>148</v>
-      </c>
       <c r="G35" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I35" s="17" t="s">
         <v>59</v>
@@ -6848,13 +6843,13 @@
         <v>59</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N35" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P35" s="17" t="s">
         <v>59</v>
@@ -6959,7 +6954,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="101" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>59</v>
@@ -6971,13 +6966,13 @@
         <v>59</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I37" s="17" t="s">
         <v>59</v>
@@ -6992,13 +6987,13 @@
         <v>59</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P37" s="17" t="s">
         <v>59</v>
@@ -7035,19 +7030,19 @@
       <c r="A38" s="48"/>
       <c r="B38" s="102"/>
       <c r="C38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>59</v>
@@ -7056,19 +7051,19 @@
         <v>59</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O38" s="17" t="s">
         <v>59</v>
@@ -7077,10 +7072,10 @@
         <v>59</v>
       </c>
       <c r="Q38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R38" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S38" s="48"/>
       <c r="T38" s="48"/>
@@ -7101,7 +7096,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="92" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>59</v>
@@ -7243,7 +7238,7 @@
         <v>15</v>
       </c>
       <c r="B41" s="92" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>59</v>
@@ -7363,7 +7358,7 @@
         <v>59</v>
       </c>
       <c r="Q42" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R42" s="17" t="s">
         <v>25</v>
@@ -7387,7 +7382,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="92" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>59</v>
@@ -8255,7 +8250,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -8265,15 +8260,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>59</v>
@@ -8281,15 +8276,15 @@
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>67</v>
@@ -8297,94 +8292,94 @@
     </row>
     <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying classes refactor add get_holidays
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -569,7 +569,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -637,8 +637,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,6 +673,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +863,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -983,6 +996,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1122,12 +1147,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1463,146 +1482,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
     <row r="2" spans="1:40" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
     </row>
     <row r="3" spans="1:40" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
     </row>
     <row r="4" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
     </row>
     <row r="5" spans="1:40" s="4" customFormat="1" ht="7.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q5" s="8"/>
-      <c r="R5" s="51" t="s">
+      <c r="R5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="52"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="84" t="s">
+      <c r="S5" s="56"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53"/>
-      <c r="Z5" s="57" t="s">
+      <c r="V5" s="56"/>
+      <c r="W5" s="57"/>
+      <c r="Z5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="50"/>
+      <c r="AA5" s="53"/>
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="54"/>
       <c r="AD5" s="26"/>
       <c r="AE5" s="26"/>
       <c r="AF5" s="26"/>
@@ -1611,116 +1630,116 @@
     </row>
     <row r="6" spans="1:40" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q6" s="8"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="56"/>
-      <c r="Z6" s="80" t="s">
+      <c r="R6" s="58"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="60"/>
+      <c r="Z6" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="AA6" s="53"/>
-      <c r="AB6" s="80" t="s">
+      <c r="AA6" s="57"/>
+      <c r="AB6" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="AC6" s="53"/>
+      <c r="AC6" s="57"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
     <row r="7" spans="1:40" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K7" s="75" t="s">
+      <c r="K7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="57">
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="61">
         <v>5</v>
       </c>
-      <c r="S7" s="49"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="66">
+      <c r="S7" s="53"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="70">
         <v>44712</v>
       </c>
-      <c r="V7" s="49"/>
-      <c r="W7" s="50"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="54"/>
       <c r="X7" s="26"/>
       <c r="Y7" s="26"/>
-      <c r="Z7" s="57" t="s">
+      <c r="Z7" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="50"/>
-      <c r="AB7" s="57" t="s">
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="50"/>
+      <c r="AC7" s="54"/>
     </row>
     <row r="8" spans="1:40" s="26" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
     </row>
     <row r="9" spans="1:40" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="86" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="48" t="s">
+      <c r="U9" s="53"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="Y9" s="49"/>
-      <c r="Z9" s="49"/>
-      <c r="AA9" s="50"/>
-      <c r="AB9" s="48" t="s">
+      <c r="Y9" s="53"/>
+      <c r="Z9" s="53"/>
+      <c r="AA9" s="54"/>
+      <c r="AB9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="AC9" s="53"/>
+      <c r="AC9" s="57"/>
     </row>
     <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68"/>
-      <c r="B10" s="68"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="16" t="s">
         <v>20</v>
       </c>
@@ -1769,37 +1788,37 @@
       <c r="R10" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="S10" s="68"/>
-      <c r="T10" s="89" t="s">
+      <c r="S10" s="72"/>
+      <c r="T10" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="89" t="s">
+      <c r="U10" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="89" t="s">
+      <c r="V10" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="87" t="s">
+      <c r="W10" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="X10" s="83" t="s">
+      <c r="X10" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="Y10" s="83" t="s">
+      <c r="Y10" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="Z10" s="83" t="s">
+      <c r="Z10" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="AA10" s="83" t="s">
+      <c r="AA10" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="AB10" s="54"/>
-      <c r="AC10" s="56"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="60"/>
     </row>
     <row r="11" spans="1:40" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="68"/>
-      <c r="B11" s="68"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="28" t="s">
         <v>41</v>
       </c>
@@ -1848,15 +1867,15 @@
       <c r="R11" s="28">
         <v>31</v>
       </c>
-      <c r="S11" s="68"/>
-      <c r="T11" s="68"/>
-      <c r="U11" s="68"/>
-      <c r="V11" s="68"/>
-      <c r="W11" s="68"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="62"/>
-      <c r="AA11" s="62"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="72"/>
+      <c r="U11" s="72"/>
+      <c r="V11" s="72"/>
+      <c r="W11" s="72"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
       <c r="AB11" s="42" t="s">
         <v>54</v>
       </c>
@@ -1874,24 +1893,24 @@
       <c r="B12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="68">
         <v>3</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="57"/>
       <c r="S12" s="34">
         <v>4</v>
       </c>
@@ -1930,10 +1949,10 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61">
+      <c r="A13" s="65">
         <v>1</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="67" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -1984,40 +2003,40 @@
       <c r="R13" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S13" s="65" t="s">
+      <c r="S13" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="T13" s="78" t="s">
+      <c r="T13" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78" t="s">
+      <c r="U13" s="82"/>
+      <c r="V13" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="W13" s="67" t="s">
+      <c r="W13" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="X13" s="67" t="s">
+      <c r="X13" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="Y13" s="67" t="s">
+      <c r="Y13" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="Z13" s="67"/>
-      <c r="AA13" s="67"/>
-      <c r="AB13" s="67" t="s">
+      <c r="Z13" s="71"/>
+      <c r="AA13" s="71"/>
+      <c r="AB13" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="AC13" s="67" t="s">
+      <c r="AC13" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="AD13" s="69" t="s">
+      <c r="AD13" s="73" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="17" t="s">
         <v>59</v>
       </c>
@@ -2066,24 +2085,24 @@
       <c r="R14" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="S14" s="62"/>
-      <c r="T14" s="68"/>
-      <c r="U14" s="68"/>
-      <c r="V14" s="68"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="68"/>
-      <c r="Y14" s="68"/>
-      <c r="Z14" s="68"/>
-      <c r="AA14" s="68"/>
-      <c r="AB14" s="68"/>
-      <c r="AC14" s="68"/>
-      <c r="AD14" s="62"/>
+      <c r="S14" s="66"/>
+      <c r="T14" s="72"/>
+      <c r="U14" s="72"/>
+      <c r="V14" s="72"/>
+      <c r="W14" s="72"/>
+      <c r="X14" s="72"/>
+      <c r="Y14" s="72"/>
+      <c r="Z14" s="72"/>
+      <c r="AA14" s="72"/>
+      <c r="AB14" s="72"/>
+      <c r="AC14" s="72"/>
+      <c r="AD14" s="66"/>
     </row>
     <row r="15" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="61">
+      <c r="A15" s="65">
         <v>2</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="67" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -2134,36 +2153,36 @@
       <c r="R15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S15" s="65" t="s">
+      <c r="S15" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="T15" s="65" t="s">
+      <c r="T15" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="U15" s="65"/>
-      <c r="V15" s="65"/>
-      <c r="W15" s="69"/>
-      <c r="X15" s="69" t="s">
+      <c r="U15" s="69"/>
+      <c r="V15" s="69"/>
+      <c r="W15" s="73"/>
+      <c r="X15" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="Y15" s="69" t="s">
+      <c r="Y15" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="Z15" s="69"/>
-      <c r="AA15" s="69"/>
-      <c r="AB15" s="69" t="s">
+      <c r="Z15" s="73"/>
+      <c r="AA15" s="73"/>
+      <c r="AB15" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="AC15" s="69" t="s">
+      <c r="AC15" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="AD15" s="69" t="s">
+      <c r="AD15" s="73" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="17" t="s">
         <v>67</v>
       </c>
@@ -2212,24 +2231,24 @@
       <c r="R16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="62"/>
-      <c r="X16" s="62"/>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="62"/>
-      <c r="AA16" s="62"/>
-      <c r="AB16" s="62"/>
-      <c r="AC16" s="62"/>
-      <c r="AD16" s="62"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="66"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="66"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="66"/>
+      <c r="AB16" s="66"/>
+      <c r="AC16" s="66"/>
+      <c r="AD16" s="66"/>
     </row>
     <row r="17" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61">
+      <c r="A17" s="65">
         <v>3</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="67" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -2280,36 +2299,36 @@
       <c r="R17" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="S17" s="70" t="s">
+      <c r="S17" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="T17" s="70" t="s">
+      <c r="T17" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="U17" s="70"/>
-      <c r="V17" s="70" t="s">
+      <c r="U17" s="74"/>
+      <c r="V17" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="W17" s="71"/>
-      <c r="X17" s="71" t="s">
+      <c r="W17" s="75"/>
+      <c r="X17" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="Y17" s="71"/>
-      <c r="Z17" s="71"/>
-      <c r="AA17" s="71"/>
-      <c r="AB17" s="71" t="s">
+      <c r="Y17" s="75"/>
+      <c r="Z17" s="75"/>
+      <c r="AA17" s="75"/>
+      <c r="AB17" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="AC17" s="71" t="s">
+      <c r="AC17" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="AD17" s="69" t="s">
+      <c r="AD17" s="73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="17" t="s">
         <v>58</v>
       </c>
@@ -2358,24 +2377,24 @@
       <c r="R18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62"/>
-      <c r="V18" s="62"/>
-      <c r="W18" s="62"/>
-      <c r="X18" s="62"/>
-      <c r="Y18" s="62"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="62"/>
-      <c r="AB18" s="62"/>
-      <c r="AC18" s="62"/>
-      <c r="AD18" s="62"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="66"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="66"/>
+      <c r="X18" s="66"/>
+      <c r="Y18" s="66"/>
+      <c r="Z18" s="66"/>
+      <c r="AA18" s="66"/>
+      <c r="AB18" s="66"/>
+      <c r="AC18" s="66"/>
+      <c r="AD18" s="66"/>
     </row>
     <row r="19" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="61">
+      <c r="A19" s="65">
         <v>4</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="67" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -2426,36 +2445,36 @@
       <c r="R19" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S19" s="65" t="s">
+      <c r="S19" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="T19" s="65" t="s">
+      <c r="T19" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="U19" s="65"/>
-      <c r="V19" s="65" t="s">
+      <c r="U19" s="69"/>
+      <c r="V19" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="W19" s="69"/>
-      <c r="X19" s="69" t="s">
+      <c r="W19" s="73"/>
+      <c r="X19" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="Y19" s="69"/>
-      <c r="Z19" s="69"/>
-      <c r="AA19" s="69"/>
-      <c r="AB19" s="69" t="s">
+      <c r="Y19" s="73"/>
+      <c r="Z19" s="73"/>
+      <c r="AA19" s="73"/>
+      <c r="AB19" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AC19" s="69" t="s">
+      <c r="AC19" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="AD19" s="69" t="s">
+      <c r="AD19" s="73" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="38" t="s">
         <v>81</v>
       </c>
@@ -2504,24 +2523,24 @@
       <c r="R20" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="62"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="62"/>
-      <c r="AD20" s="62"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
+      <c r="U20" s="66"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="66"/>
+      <c r="X20" s="66"/>
+      <c r="Y20" s="66"/>
+      <c r="Z20" s="66"/>
+      <c r="AA20" s="66"/>
+      <c r="AB20" s="66"/>
+      <c r="AC20" s="66"/>
+      <c r="AD20" s="66"/>
     </row>
     <row r="21" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="61">
+      <c r="A21" s="65">
         <v>5</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="67" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -2572,38 +2591,38 @@
       <c r="R21" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S21" s="65" t="s">
+      <c r="S21" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="T21" s="78" t="s">
+      <c r="T21" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="U21" s="78"/>
-      <c r="V21" s="78" t="s">
+      <c r="U21" s="82"/>
+      <c r="V21" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="W21" s="67" t="s">
+      <c r="W21" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="X21" s="67" t="s">
+      <c r="X21" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="Y21" s="67"/>
-      <c r="Z21" s="67"/>
-      <c r="AA21" s="67"/>
-      <c r="AB21" s="67" t="s">
+      <c r="Y21" s="71"/>
+      <c r="Z21" s="71"/>
+      <c r="AA21" s="71"/>
+      <c r="AB21" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="AC21" s="67" t="s">
+      <c r="AC21" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="AD21" s="69" t="s">
+      <c r="AD21" s="73" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
-      <c r="B22" s="62"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="17" t="s">
         <v>59</v>
       </c>
@@ -2652,24 +2671,24 @@
       <c r="R22" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S22" s="62"/>
-      <c r="T22" s="68"/>
-      <c r="U22" s="68"/>
-      <c r="V22" s="68"/>
-      <c r="W22" s="68"/>
-      <c r="X22" s="68"/>
-      <c r="Y22" s="68"/>
-      <c r="Z22" s="68"/>
-      <c r="AA22" s="68"/>
-      <c r="AB22" s="68"/>
-      <c r="AC22" s="68"/>
-      <c r="AD22" s="62"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="72"/>
+      <c r="U22" s="72"/>
+      <c r="V22" s="72"/>
+      <c r="W22" s="72"/>
+      <c r="X22" s="72"/>
+      <c r="Y22" s="72"/>
+      <c r="Z22" s="72"/>
+      <c r="AA22" s="72"/>
+      <c r="AB22" s="72"/>
+      <c r="AC22" s="72"/>
+      <c r="AD22" s="66"/>
     </row>
     <row r="23" spans="1:30" s="15" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="72">
+      <c r="A23" s="76">
         <v>6</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="67" t="s">
         <v>85</v>
       </c>
       <c r="C23" s="17" t="s">
@@ -2720,36 +2739,36 @@
       <c r="R23" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S23" s="65" t="s">
+      <c r="S23" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="T23" s="65" t="s">
+      <c r="T23" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="U23" s="65"/>
-      <c r="V23" s="65" t="s">
+      <c r="U23" s="69"/>
+      <c r="V23" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="W23" s="69"/>
-      <c r="X23" s="69" t="s">
+      <c r="W23" s="73"/>
+      <c r="X23" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="Y23" s="69"/>
-      <c r="Z23" s="69"/>
-      <c r="AA23" s="69"/>
-      <c r="AB23" s="69" t="s">
+      <c r="Y23" s="73"/>
+      <c r="Z23" s="73"/>
+      <c r="AA23" s="73"/>
+      <c r="AB23" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AC23" s="69" t="s">
+      <c r="AC23" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="AD23" s="69" t="s">
+      <c r="AD23" s="73" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:30" s="15" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="62"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="38" t="s">
         <v>81</v>
       </c>
@@ -2798,24 +2817,24 @@
       <c r="R24" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="62"/>
-      <c r="Y24" s="62"/>
-      <c r="Z24" s="62"/>
-      <c r="AA24" s="62"/>
-      <c r="AB24" s="62"/>
-      <c r="AC24" s="62"/>
-      <c r="AD24" s="62"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
+      <c r="U24" s="66"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="66"/>
+      <c r="X24" s="66"/>
+      <c r="Y24" s="66"/>
+      <c r="Z24" s="66"/>
+      <c r="AA24" s="66"/>
+      <c r="AB24" s="66"/>
+      <c r="AC24" s="66"/>
+      <c r="AD24" s="66"/>
     </row>
     <row r="25" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="61">
+      <c r="A25" s="65">
         <v>7</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="67" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="17" t="s">
@@ -2866,38 +2885,38 @@
       <c r="R25" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S25" s="65" t="s">
+      <c r="S25" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="T25" s="65" t="s">
+      <c r="T25" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="U25" s="65"/>
-      <c r="V25" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="W25" s="65"/>
-      <c r="X25" s="69" t="s">
+      <c r="U25" s="69"/>
+      <c r="V25" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="W25" s="69"/>
+      <c r="X25" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="Y25" s="69" t="s">
+      <c r="Y25" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="Z25" s="69"/>
-      <c r="AA25" s="69"/>
-      <c r="AB25" s="69" t="s">
+      <c r="Z25" s="73"/>
+      <c r="AA25" s="73"/>
+      <c r="AB25" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="AC25" s="69" t="s">
+      <c r="AC25" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="AD25" s="69" t="s">
+      <c r="AD25" s="73" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="62"/>
-      <c r="B26" s="62"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="17" t="s">
         <v>67</v>
       </c>
@@ -2946,24 +2965,24 @@
       <c r="R26" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="S26" s="62"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="62"/>
-      <c r="V26" s="62"/>
-      <c r="W26" s="62"/>
-      <c r="X26" s="62"/>
-      <c r="Y26" s="62"/>
-      <c r="Z26" s="62"/>
-      <c r="AA26" s="62"/>
-      <c r="AB26" s="62"/>
-      <c r="AC26" s="62"/>
-      <c r="AD26" s="62"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="66"/>
+      <c r="U26" s="66"/>
+      <c r="V26" s="66"/>
+      <c r="W26" s="66"/>
+      <c r="X26" s="66"/>
+      <c r="Y26" s="66"/>
+      <c r="Z26" s="66"/>
+      <c r="AA26" s="66"/>
+      <c r="AB26" s="66"/>
+      <c r="AC26" s="66"/>
+      <c r="AD26" s="66"/>
     </row>
     <row r="27" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61">
+      <c r="A27" s="65">
         <v>8</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="67" t="s">
         <v>90</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -3014,38 +3033,38 @@
       <c r="R27" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S27" s="65" t="s">
+      <c r="S27" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="T27" s="65" t="s">
+      <c r="T27" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="U27" s="65"/>
-      <c r="V27" s="65" t="s">
+      <c r="U27" s="69"/>
+      <c r="V27" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="W27" s="65" t="s">
+      <c r="W27" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="X27" s="69" t="s">
+      <c r="X27" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="Y27" s="69"/>
-      <c r="Z27" s="69"/>
-      <c r="AA27" s="69"/>
-      <c r="AB27" s="69" t="s">
+      <c r="Y27" s="73"/>
+      <c r="Z27" s="73"/>
+      <c r="AA27" s="73"/>
+      <c r="AB27" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="AC27" s="69" t="s">
+      <c r="AC27" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="AD27" s="69" t="s">
+      <c r="AD27" s="73" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="62"/>
-      <c r="B28" s="62"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="66"/>
       <c r="C28" s="18" t="s">
         <v>60</v>
       </c>
@@ -3094,24 +3113,24 @@
       <c r="R28" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="S28" s="62"/>
-      <c r="T28" s="62"/>
-      <c r="U28" s="62"/>
-      <c r="V28" s="62"/>
-      <c r="W28" s="62"/>
-      <c r="X28" s="62"/>
-      <c r="Y28" s="62"/>
-      <c r="Z28" s="62"/>
-      <c r="AA28" s="62"/>
-      <c r="AB28" s="62"/>
-      <c r="AC28" s="62"/>
-      <c r="AD28" s="62"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="66"/>
+      <c r="W28" s="66"/>
+      <c r="X28" s="66"/>
+      <c r="Y28" s="66"/>
+      <c r="Z28" s="66"/>
+      <c r="AA28" s="66"/>
+      <c r="AB28" s="66"/>
+      <c r="AC28" s="66"/>
+      <c r="AD28" s="66"/>
     </row>
     <row r="29" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="61">
+      <c r="A29" s="65">
         <v>9</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="67" t="s">
         <v>95</v>
       </c>
       <c r="C29" s="17" t="s">
@@ -3162,38 +3181,38 @@
       <c r="R29" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="S29" s="70" t="s">
+      <c r="S29" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="T29" s="70" t="s">
+      <c r="T29" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="U29" s="70"/>
-      <c r="V29" s="70" t="s">
+      <c r="U29" s="74"/>
+      <c r="V29" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="W29" s="71"/>
-      <c r="X29" s="71" t="s">
+      <c r="W29" s="75"/>
+      <c r="X29" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="Y29" s="71" t="s">
+      <c r="Y29" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="Z29" s="71"/>
-      <c r="AA29" s="71"/>
-      <c r="AB29" s="71" t="s">
+      <c r="Z29" s="75"/>
+      <c r="AA29" s="75"/>
+      <c r="AB29" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="AC29" s="71" t="s">
+      <c r="AC29" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="AD29" s="69" t="s">
+      <c r="AD29" s="73" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="62"/>
-      <c r="B30" s="62"/>
+      <c r="A30" s="66"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="17" t="s">
         <v>58</v>
       </c>
@@ -3242,24 +3261,24 @@
       <c r="R30" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="S30" s="62"/>
-      <c r="T30" s="62"/>
-      <c r="U30" s="62"/>
-      <c r="V30" s="62"/>
-      <c r="W30" s="62"/>
-      <c r="X30" s="62"/>
-      <c r="Y30" s="62"/>
-      <c r="Z30" s="62"/>
-      <c r="AA30" s="62"/>
-      <c r="AB30" s="62"/>
-      <c r="AC30" s="62"/>
-      <c r="AD30" s="62"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="66"/>
+      <c r="X30" s="66"/>
+      <c r="Y30" s="66"/>
+      <c r="Z30" s="66"/>
+      <c r="AA30" s="66"/>
+      <c r="AB30" s="66"/>
+      <c r="AC30" s="66"/>
+      <c r="AD30" s="66"/>
     </row>
     <row r="31" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="61">
+      <c r="A31" s="65">
         <v>10</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="67" t="s">
         <v>101</v>
       </c>
       <c r="C31" s="38" t="s">
@@ -3310,36 +3329,36 @@
       <c r="R31" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="S31" s="90" t="s">
+      <c r="S31" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="T31" s="90" t="s">
+      <c r="T31" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="U31" s="90"/>
-      <c r="V31" s="90" t="s">
+      <c r="U31" s="94"/>
+      <c r="V31" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="W31" s="90"/>
-      <c r="X31" s="88" t="s">
+      <c r="W31" s="94"/>
+      <c r="X31" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="Y31" s="88"/>
-      <c r="Z31" s="88"/>
-      <c r="AA31" s="88"/>
-      <c r="AB31" s="88" t="s">
+      <c r="Y31" s="92"/>
+      <c r="Z31" s="92"/>
+      <c r="AA31" s="92"/>
+      <c r="AB31" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="AC31" s="69" t="s">
+      <c r="AC31" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="AD31" s="69" t="s">
+      <c r="AD31" s="73" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="62"/>
-      <c r="B32" s="62"/>
+      <c r="A32" s="66"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="38" t="s">
         <v>25</v>
       </c>
@@ -3388,24 +3407,24 @@
       <c r="R32" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="S32" s="62"/>
-      <c r="T32" s="62"/>
-      <c r="U32" s="62"/>
-      <c r="V32" s="62"/>
-      <c r="W32" s="62"/>
-      <c r="X32" s="62"/>
-      <c r="Y32" s="62"/>
-      <c r="Z32" s="62"/>
-      <c r="AA32" s="62"/>
-      <c r="AB32" s="62"/>
-      <c r="AC32" s="62"/>
-      <c r="AD32" s="62"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="66"/>
+      <c r="U32" s="66"/>
+      <c r="V32" s="66"/>
+      <c r="W32" s="66"/>
+      <c r="X32" s="66"/>
+      <c r="Y32" s="66"/>
+      <c r="Z32" s="66"/>
+      <c r="AA32" s="66"/>
+      <c r="AB32" s="66"/>
+      <c r="AC32" s="66"/>
+      <c r="AD32" s="66"/>
     </row>
     <row r="33" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="61">
+      <c r="A33" s="65">
         <v>11</v>
       </c>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="67" t="s">
         <v>104</v>
       </c>
       <c r="C33" s="17" t="s">
@@ -3456,38 +3475,38 @@
       <c r="R33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S33" s="70" t="s">
+      <c r="S33" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="T33" s="65" t="s">
+      <c r="T33" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="U33" s="65"/>
-      <c r="V33" s="65" t="s">
+      <c r="U33" s="69"/>
+      <c r="V33" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="W33" s="65" t="s">
+      <c r="W33" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="X33" s="69" t="s">
+      <c r="X33" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="Y33" s="69"/>
-      <c r="Z33" s="69"/>
-      <c r="AA33" s="69"/>
-      <c r="AB33" s="69" t="s">
+      <c r="Y33" s="73"/>
+      <c r="Z33" s="73"/>
+      <c r="AA33" s="73"/>
+      <c r="AB33" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="AC33" s="71" t="s">
+      <c r="AC33" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="AD33" s="71" t="s">
+      <c r="AD33" s="75" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="62"/>
-      <c r="B34" s="62"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="18" t="s">
         <v>60</v>
       </c>
@@ -3536,24 +3555,24 @@
       <c r="R34" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="S34" s="62"/>
-      <c r="T34" s="62"/>
-      <c r="U34" s="62"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="62"/>
-      <c r="X34" s="62"/>
-      <c r="Y34" s="62"/>
-      <c r="Z34" s="62"/>
-      <c r="AA34" s="62"/>
-      <c r="AB34" s="62"/>
-      <c r="AC34" s="62"/>
-      <c r="AD34" s="62"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="66"/>
+      <c r="U34" s="66"/>
+      <c r="V34" s="66"/>
+      <c r="W34" s="66"/>
+      <c r="X34" s="66"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="66"/>
+      <c r="AA34" s="66"/>
+      <c r="AB34" s="66"/>
+      <c r="AC34" s="66"/>
+      <c r="AD34" s="66"/>
     </row>
     <row r="35" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="61">
+      <c r="A35" s="65">
         <v>12</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="67" t="s">
         <v>105</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -3604,30 +3623,30 @@
       <c r="R35" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S35" s="65" t="s">
+      <c r="S35" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="T35" s="69" t="s">
+      <c r="T35" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="U35" s="65"/>
-      <c r="V35" s="65"/>
-      <c r="W35" s="65"/>
-      <c r="X35" s="69" t="s">
+      <c r="U35" s="69"/>
+      <c r="V35" s="69"/>
+      <c r="W35" s="69"/>
+      <c r="X35" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="Y35" s="69" t="s">
+      <c r="Y35" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="Z35" s="69"/>
-      <c r="AA35" s="69"/>
-      <c r="AB35" s="69"/>
-      <c r="AC35" s="69"/>
-      <c r="AD35" s="69"/>
+      <c r="Z35" s="73"/>
+      <c r="AA35" s="73"/>
+      <c r="AB35" s="73"/>
+      <c r="AC35" s="73"/>
+      <c r="AD35" s="73"/>
     </row>
     <row r="36" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="62"/>
-      <c r="B36" s="62"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="38" t="s">
         <v>67</v>
       </c>
@@ -3676,24 +3695,24 @@
       <c r="R36" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="S36" s="62"/>
-      <c r="T36" s="62"/>
-      <c r="U36" s="62"/>
-      <c r="V36" s="62"/>
-      <c r="W36" s="62"/>
-      <c r="X36" s="62"/>
-      <c r="Y36" s="62"/>
-      <c r="Z36" s="62"/>
-      <c r="AA36" s="62"/>
-      <c r="AB36" s="62"/>
-      <c r="AC36" s="62"/>
-      <c r="AD36" s="62"/>
+      <c r="S36" s="66"/>
+      <c r="T36" s="66"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="66"/>
+      <c r="W36" s="66"/>
+      <c r="X36" s="66"/>
+      <c r="Y36" s="66"/>
+      <c r="Z36" s="66"/>
+      <c r="AA36" s="66"/>
+      <c r="AB36" s="66"/>
+      <c r="AC36" s="66"/>
+      <c r="AD36" s="66"/>
     </row>
     <row r="37" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="61">
+      <c r="A37" s="65">
         <v>13</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="67" t="s">
         <v>106</v>
       </c>
       <c r="C37" s="17" t="s">
@@ -3744,28 +3763,28 @@
       <c r="R37" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S37" s="65" t="s">
+      <c r="S37" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="T37" s="69" t="s">
+      <c r="T37" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="U37" s="65"/>
-      <c r="V37" s="65"/>
-      <c r="W37" s="65"/>
-      <c r="X37" s="69" t="s">
+      <c r="U37" s="69"/>
+      <c r="V37" s="69"/>
+      <c r="W37" s="69"/>
+      <c r="X37" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="Y37" s="69"/>
-      <c r="Z37" s="69"/>
-      <c r="AA37" s="69"/>
-      <c r="AB37" s="69"/>
-      <c r="AC37" s="69"/>
-      <c r="AD37" s="69"/>
+      <c r="Y37" s="73"/>
+      <c r="Z37" s="73"/>
+      <c r="AA37" s="73"/>
+      <c r="AB37" s="73"/>
+      <c r="AC37" s="73"/>
+      <c r="AD37" s="73"/>
     </row>
     <row r="38" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="62"/>
-      <c r="B38" s="62"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="17" t="s">
         <v>25</v>
       </c>
@@ -3814,24 +3833,24 @@
       <c r="R38" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S38" s="62"/>
-      <c r="T38" s="62"/>
-      <c r="U38" s="62"/>
-      <c r="V38" s="62"/>
-      <c r="W38" s="62"/>
-      <c r="X38" s="62"/>
-      <c r="Y38" s="62"/>
-      <c r="Z38" s="62"/>
-      <c r="AA38" s="62"/>
-      <c r="AB38" s="62"/>
-      <c r="AC38" s="62"/>
-      <c r="AD38" s="62"/>
+      <c r="S38" s="66"/>
+      <c r="T38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="66"/>
+      <c r="Y38" s="66"/>
+      <c r="Z38" s="66"/>
+      <c r="AA38" s="66"/>
+      <c r="AB38" s="66"/>
+      <c r="AC38" s="66"/>
+      <c r="AD38" s="66"/>
     </row>
     <row r="39" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="61">
+      <c r="A39" s="65">
         <v>14</v>
       </c>
-      <c r="B39" s="63" t="s">
+      <c r="B39" s="67" t="s">
         <v>107</v>
       </c>
       <c r="C39" s="17" t="s">
@@ -3882,28 +3901,28 @@
       <c r="R39" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S39" s="65" t="s">
+      <c r="S39" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="T39" s="69" t="s">
+      <c r="T39" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="U39" s="65"/>
-      <c r="V39" s="65"/>
-      <c r="W39" s="65"/>
-      <c r="X39" s="69" t="s">
+      <c r="U39" s="69"/>
+      <c r="V39" s="69"/>
+      <c r="W39" s="69"/>
+      <c r="X39" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="Y39" s="69"/>
-      <c r="Z39" s="69"/>
-      <c r="AA39" s="69"/>
-      <c r="AB39" s="69"/>
-      <c r="AC39" s="69"/>
-      <c r="AD39" s="69"/>
+      <c r="Y39" s="73"/>
+      <c r="Z39" s="73"/>
+      <c r="AA39" s="73"/>
+      <c r="AB39" s="73"/>
+      <c r="AC39" s="73"/>
+      <c r="AD39" s="73"/>
     </row>
     <row r="40" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="62"/>
-      <c r="B40" s="62"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="17" t="s">
         <v>25</v>
       </c>
@@ -3952,18 +3971,18 @@
       <c r="R40" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S40" s="62"/>
-      <c r="T40" s="62"/>
-      <c r="U40" s="62"/>
-      <c r="V40" s="62"/>
-      <c r="W40" s="62"/>
-      <c r="X40" s="62"/>
-      <c r="Y40" s="62"/>
-      <c r="Z40" s="62"/>
-      <c r="AA40" s="62"/>
-      <c r="AB40" s="62"/>
-      <c r="AC40" s="62"/>
-      <c r="AD40" s="62"/>
+      <c r="S40" s="66"/>
+      <c r="T40" s="66"/>
+      <c r="U40" s="66"/>
+      <c r="V40" s="66"/>
+      <c r="W40" s="66"/>
+      <c r="X40" s="66"/>
+      <c r="Y40" s="66"/>
+      <c r="Z40" s="66"/>
+      <c r="AA40" s="66"/>
+      <c r="AB40" s="66"/>
+      <c r="AC40" s="66"/>
+      <c r="AD40" s="66"/>
     </row>
     <row r="41" spans="1:30" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
@@ -3998,31 +4017,31 @@
       <c r="AD41" s="12"/>
     </row>
     <row r="42" spans="1:30" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="73" t="s">
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-      <c r="M42" s="59"/>
-      <c r="N42" s="55"/>
-      <c r="O42" s="55"/>
-      <c r="Q42" s="59" t="s">
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="Q42" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="R42" s="55"/>
-      <c r="S42" s="55"/>
-      <c r="T42" s="55"/>
-      <c r="U42" s="55"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="59"/>
       <c r="V42" s="4"/>
       <c r="W42" s="4" t="s">
         <v>111</v>
@@ -4036,31 +4055,31 @@
       <c r="AD42" s="12"/>
     </row>
     <row r="43" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="47"/>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="74" t="s">
+      <c r="A43" s="51"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="52"/>
-      <c r="M43" s="60" t="s">
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="56"/>
+      <c r="M43" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="N43" s="52"/>
-      <c r="O43" s="52"/>
-      <c r="Q43" s="60" t="s">
+      <c r="N43" s="56"/>
+      <c r="O43" s="56"/>
+      <c r="Q43" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="R43" s="52"/>
-      <c r="S43" s="52"/>
-      <c r="T43" s="52"/>
-      <c r="U43" s="52"/>
+      <c r="R43" s="56"/>
+      <c r="S43" s="56"/>
+      <c r="T43" s="56"/>
+      <c r="U43" s="56"/>
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
@@ -4072,31 +4091,31 @@
       <c r="AD43" s="12"/>
     </row>
     <row r="44" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="58" t="s">
+      <c r="A44" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="73" t="s">
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="M44" s="59"/>
-      <c r="N44" s="55"/>
-      <c r="O44" s="55"/>
-      <c r="Q44" s="59" t="s">
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="Q44" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="R44" s="55"/>
-      <c r="S44" s="55"/>
-      <c r="T44" s="55"/>
-      <c r="U44" s="55"/>
+      <c r="R44" s="59"/>
+      <c r="S44" s="59"/>
+      <c r="T44" s="59"/>
+      <c r="U44" s="59"/>
       <c r="V44" s="4"/>
       <c r="W44" s="4" t="s">
         <v>111</v>
@@ -4110,31 +4129,31 @@
       <c r="AD44" s="4"/>
     </row>
     <row r="45" spans="1:30" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="47"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="74" t="s">
+      <c r="A45" s="51"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="F45" s="52"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="52"/>
-      <c r="M45" s="60" t="s">
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="M45" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="N45" s="52"/>
-      <c r="O45" s="52"/>
-      <c r="Q45" s="60" t="s">
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="Q45" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="R45" s="52"/>
-      <c r="S45" s="52"/>
-      <c r="T45" s="52"/>
-      <c r="U45" s="52"/>
+      <c r="R45" s="56"/>
+      <c r="S45" s="56"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
@@ -4146,31 +4165,31 @@
       <c r="AD45" s="4"/>
     </row>
     <row r="46" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="73" t="s">
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="M46" s="59"/>
-      <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="Q46" s="59" t="s">
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="59"/>
+      <c r="O46" s="59"/>
+      <c r="Q46" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="R46" s="55"/>
-      <c r="S46" s="55"/>
-      <c r="T46" s="55"/>
-      <c r="U46" s="55"/>
+      <c r="R46" s="59"/>
+      <c r="S46" s="59"/>
+      <c r="T46" s="59"/>
+      <c r="U46" s="59"/>
       <c r="V46" s="4"/>
       <c r="W46" s="4" t="s">
         <v>111</v>
@@ -4184,31 +4203,31 @@
       <c r="AD46" s="4"/>
     </row>
     <row r="47" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="47"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="77" t="s">
+      <c r="A47" s="51"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
-      <c r="M47" s="46" t="s">
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="M47" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="N47" s="47"/>
-      <c r="O47" s="47"/>
-      <c r="Q47" s="60" t="s">
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="Q47" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="R47" s="52"/>
-      <c r="S47" s="52"/>
-      <c r="T47" s="52"/>
-      <c r="U47" s="52"/>
+      <c r="R47" s="56"/>
+      <c r="S47" s="56"/>
+      <c r="T47" s="56"/>
+      <c r="U47" s="56"/>
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
@@ -4640,7 +4659,7 @@
   <dimension ref="A1:AO56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4664,149 +4683,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
     </row>
     <row r="2" spans="1:41" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
     </row>
     <row r="3" spans="1:41" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
     </row>
     <row r="4" spans="1:41" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="86"/>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
     </row>
     <row r="5" spans="1:41" s="4" customFormat="1" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q5" s="8"/>
-      <c r="R5" s="51" t="s">
+      <c r="R5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="52"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="84" t="s">
+      <c r="S5" s="56"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="52"/>
-      <c r="W5" s="53"/>
-      <c r="Z5" s="57" t="s">
+      <c r="V5" s="56"/>
+      <c r="W5" s="57"/>
+      <c r="Z5" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="50"/>
+      <c r="AA5" s="53"/>
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="53"/>
+      <c r="AD5" s="54"/>
       <c r="AE5" s="26"/>
       <c r="AF5" s="26"/>
       <c r="AG5" s="26"/>
@@ -4815,67 +4834,67 @@
     </row>
     <row r="6" spans="1:41" s="4" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q6" s="8"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="56"/>
-      <c r="Z6" s="80" t="s">
+      <c r="R6" s="58"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="60"/>
+      <c r="Z6" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="AA6" s="52"/>
-      <c r="AB6" s="53"/>
-      <c r="AC6" s="80" t="s">
+      <c r="AA6" s="56"/>
+      <c r="AB6" s="57"/>
+      <c r="AC6" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="AD6" s="53"/>
+      <c r="AD6" s="57"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
     </row>
     <row r="7" spans="1:41" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K7" s="75" t="s">
+      <c r="K7" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="92">
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="96">
         <v>5</v>
       </c>
-      <c r="S7" s="49"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="93">
+      <c r="S7" s="53"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="97">
         <v>44712</v>
       </c>
-      <c r="V7" s="49"/>
-      <c r="W7" s="50"/>
-      <c r="Z7" s="92" t="s">
+      <c r="V7" s="53"/>
+      <c r="W7" s="54"/>
+      <c r="Z7" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="49"/>
-      <c r="AB7" s="50"/>
-      <c r="AC7" s="92" t="s">
+      <c r="AA7" s="53"/>
+      <c r="AB7" s="54"/>
+      <c r="AC7" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="AD7" s="50"/>
+      <c r="AD7" s="54"/>
     </row>
     <row r="8" spans="1:41" s="26" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
       <c r="AF8" s="32" t="s">
         <v>121</v>
       </c>
@@ -4884,136 +4903,136 @@
       </c>
     </row>
     <row r="9" spans="1:41" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="48" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="54"/>
+      <c r="S9" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="48" t="s">
+      <c r="U9" s="53"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="54"/>
+      <c r="X9" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="Y9" s="49"/>
-      <c r="Z9" s="49"/>
-      <c r="AA9" s="49"/>
-      <c r="AB9" s="50"/>
-      <c r="AC9" s="48" t="s">
+      <c r="Y9" s="53"/>
+      <c r="Z9" s="53"/>
+      <c r="AA9" s="53"/>
+      <c r="AB9" s="54"/>
+      <c r="AC9" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="AD9" s="53"/>
+      <c r="AD9" s="57"/>
       <c r="AE9" s="31"/>
       <c r="AF9" s="32" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:41" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="68"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="101" t="s">
+      <c r="A10" s="72"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="E10" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="102" t="s">
+      <c r="G10" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="102" t="s">
+      <c r="H10" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="I10" s="101" t="s">
+      <c r="I10" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="101" t="s">
+      <c r="J10" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="101" t="s">
+      <c r="L10" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="102" t="s">
+      <c r="M10" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="N10" s="102" t="s">
+      <c r="N10" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="102" t="s">
+      <c r="O10" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="101" t="s">
+      <c r="P10" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="Q10" s="101">
+      <c r="Q10" s="46">
         <v>15</v>
       </c>
-      <c r="R10" s="102" t="s">
+      <c r="R10" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="S10" s="68"/>
-      <c r="T10" s="91" t="s">
+      <c r="S10" s="72"/>
+      <c r="T10" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="91" t="s">
+      <c r="U10" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="91" t="s">
+      <c r="V10" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="83" t="s">
+      <c r="W10" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="X10" s="83" t="s">
+      <c r="X10" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="Y10" s="83" t="s">
+      <c r="Y10" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="Z10" s="83" t="s">
+      <c r="Z10" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="AA10" s="83" t="s">
+      <c r="AA10" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="AB10" s="83" t="s">
+      <c r="AB10" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="AC10" s="54"/>
-      <c r="AD10" s="56"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="60"/>
       <c r="AE10" s="30"/>
       <c r="AF10" s="32" t="s">
         <v>125</v>
@@ -5023,70 +5042,70 @@
       </c>
     </row>
     <row r="11" spans="1:41" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="102" t="s">
+      <c r="A11" s="66"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="102" t="s">
+      <c r="D11" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="102" t="s">
+      <c r="E11" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="102" t="s">
+      <c r="F11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="102" t="s">
+      <c r="G11" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="101" t="s">
+      <c r="H11" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="101" t="s">
+      <c r="I11" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="102" t="s">
+      <c r="J11" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="102" t="s">
+      <c r="K11" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="102" t="s">
+      <c r="L11" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="102" t="s">
+      <c r="M11" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="102" t="s">
+      <c r="N11" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="101" t="s">
+      <c r="O11" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="P11" s="101">
+      <c r="P11" s="46">
         <v>29</v>
       </c>
-      <c r="Q11" s="102">
+      <c r="Q11" s="49">
         <v>30</v>
       </c>
-      <c r="R11" s="102">
+      <c r="R11" s="49">
         <v>31</v>
       </c>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="62"/>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="62"/>
-      <c r="AC11" s="83" t="s">
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
+      <c r="Z11" s="66"/>
+      <c r="AA11" s="66"/>
+      <c r="AB11" s="66"/>
+      <c r="AC11" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="AD11" s="83" t="s">
+      <c r="AD11" s="87" t="s">
         <v>55</v>
       </c>
       <c r="AE11" s="41" t="s">
@@ -5101,24 +5120,24 @@
       <c r="B12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="68">
         <v>3</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="57"/>
       <c r="S12" s="34">
         <v>4</v>
       </c>
@@ -5158,10 +5177,10 @@
       </c>
     </row>
     <row r="13" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61">
+      <c r="A13" s="65">
         <v>1</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="67" t="s">
         <v>126</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -5212,39 +5231,39 @@
       <c r="R13" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S13" s="65">
+      <c r="S13" s="69">
         <v>20</v>
       </c>
-      <c r="T13" s="65">
+      <c r="T13" s="69">
         <v>192</v>
       </c>
-      <c r="U13" s="65"/>
-      <c r="V13" s="65">
+      <c r="U13" s="69"/>
+      <c r="V13" s="69">
         <v>64</v>
       </c>
-      <c r="W13" s="65">
+      <c r="W13" s="69">
         <v>36</v>
       </c>
-      <c r="X13" s="69">
+      <c r="X13" s="73">
         <v>11</v>
       </c>
-      <c r="Y13" s="69"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="69"/>
-      <c r="AB13" s="69"/>
-      <c r="AC13" s="69" t="s">
+      <c r="Y13" s="73"/>
+      <c r="Z13" s="73"/>
+      <c r="AA13" s="73"/>
+      <c r="AB13" s="73"/>
+      <c r="AC13" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AD13" s="69" t="s">
+      <c r="AD13" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AE13" s="69" t="s">
+      <c r="AE13" s="73" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="17" t="s">
         <v>59</v>
       </c>
@@ -5291,27 +5310,27 @@
         <v>67</v>
       </c>
       <c r="R14" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="S14" s="62"/>
-      <c r="T14" s="62"/>
-      <c r="U14" s="62"/>
-      <c r="V14" s="62"/>
-      <c r="W14" s="62"/>
-      <c r="X14" s="62"/>
-      <c r="Y14" s="62"/>
-      <c r="Z14" s="62"/>
-      <c r="AA14" s="62"/>
-      <c r="AB14" s="62"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="62"/>
-      <c r="AE14" s="62"/>
+        <v>25</v>
+      </c>
+      <c r="S14" s="66"/>
+      <c r="T14" s="66"/>
+      <c r="U14" s="66"/>
+      <c r="V14" s="66"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="66"/>
+      <c r="Y14" s="66"/>
+      <c r="Z14" s="66"/>
+      <c r="AA14" s="66"/>
+      <c r="AB14" s="66"/>
+      <c r="AC14" s="66"/>
+      <c r="AD14" s="66"/>
+      <c r="AE14" s="66"/>
     </row>
     <row r="15" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="61">
+      <c r="A15" s="65">
         <v>2</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="67" t="s">
         <v>129</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -5362,39 +5381,39 @@
       <c r="R15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S15" s="65">
+      <c r="S15" s="69">
         <v>17</v>
       </c>
-      <c r="T15" s="65">
+      <c r="T15" s="69">
         <v>160</v>
       </c>
-      <c r="U15" s="65"/>
-      <c r="V15" s="65">
+      <c r="U15" s="69"/>
+      <c r="V15" s="69">
         <v>42</v>
       </c>
-      <c r="W15" s="69">
+      <c r="W15" s="73">
         <v>8</v>
       </c>
-      <c r="X15" s="69">
+      <c r="X15" s="73">
         <v>14</v>
       </c>
-      <c r="Y15" s="69"/>
-      <c r="Z15" s="69"/>
+      <c r="Y15" s="73"/>
+      <c r="Z15" s="73"/>
       <c r="AA15" s="37"/>
-      <c r="AB15" s="69"/>
-      <c r="AC15" s="69" t="s">
+      <c r="AB15" s="73"/>
+      <c r="AC15" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="AD15" s="69" t="s">
+      <c r="AD15" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="AE15" s="99" t="s">
+      <c r="AE15" s="103" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:41" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="20" t="s">
         <v>81</v>
       </c>
@@ -5443,25 +5462,25 @@
       <c r="R16" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="62"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="62"/>
-      <c r="X16" s="62"/>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="62"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="66"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="66"/>
+      <c r="Z16" s="66"/>
       <c r="AA16" s="39"/>
-      <c r="AB16" s="62"/>
-      <c r="AC16" s="62"/>
-      <c r="AD16" s="62"/>
-      <c r="AE16" s="100"/>
+      <c r="AB16" s="66"/>
+      <c r="AC16" s="66"/>
+      <c r="AD16" s="66"/>
+      <c r="AE16" s="104"/>
     </row>
     <row r="17" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61">
+      <c r="A17" s="65">
         <v>3</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="67" t="s">
         <v>131</v>
       </c>
       <c r="C17" s="38" t="s">
@@ -5512,41 +5531,41 @@
       <c r="R17" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S17" s="65">
+      <c r="S17" s="69">
         <v>13</v>
       </c>
-      <c r="T17" s="65">
+      <c r="T17" s="69">
         <v>128</v>
       </c>
-      <c r="U17" s="65"/>
-      <c r="V17" s="65">
+      <c r="U17" s="69"/>
+      <c r="V17" s="69">
         <v>48</v>
       </c>
-      <c r="W17" s="69">
+      <c r="W17" s="73">
         <v>12</v>
       </c>
-      <c r="X17" s="69">
+      <c r="X17" s="73">
         <v>9</v>
       </c>
-      <c r="Y17" s="69"/>
-      <c r="Z17" s="69">
+      <c r="Y17" s="73"/>
+      <c r="Z17" s="73">
         <v>9</v>
       </c>
-      <c r="AA17" s="69"/>
-      <c r="AB17" s="69"/>
-      <c r="AC17" s="69" t="s">
+      <c r="AA17" s="73"/>
+      <c r="AB17" s="73"/>
+      <c r="AC17" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="AD17" s="69" t="s">
+      <c r="AD17" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="AE17" s="69" t="s">
+      <c r="AE17" s="73" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="17" t="s">
         <v>58</v>
       </c>
@@ -5595,25 +5614,25 @@
       <c r="R18" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62"/>
-      <c r="V18" s="62"/>
-      <c r="W18" s="62"/>
-      <c r="X18" s="62"/>
-      <c r="Y18" s="62"/>
-      <c r="Z18" s="62"/>
-      <c r="AA18" s="62"/>
-      <c r="AB18" s="62"/>
-      <c r="AC18" s="62"/>
-      <c r="AD18" s="62"/>
-      <c r="AE18" s="62"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="66"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="66"/>
+      <c r="X18" s="66"/>
+      <c r="Y18" s="66"/>
+      <c r="Z18" s="66"/>
+      <c r="AA18" s="66"/>
+      <c r="AB18" s="66"/>
+      <c r="AC18" s="66"/>
+      <c r="AD18" s="66"/>
+      <c r="AE18" s="66"/>
     </row>
     <row r="19" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="61">
+      <c r="A19" s="65">
         <v>4</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="67" t="s">
         <v>135</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -5664,39 +5683,39 @@
       <c r="R19" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S19" s="65">
+      <c r="S19" s="69">
         <v>20</v>
       </c>
-      <c r="T19" s="65">
+      <c r="T19" s="69">
         <v>200</v>
       </c>
-      <c r="U19" s="65"/>
-      <c r="V19" s="65">
+      <c r="U19" s="69"/>
+      <c r="V19" s="69">
         <v>62</v>
       </c>
-      <c r="W19" s="65">
+      <c r="W19" s="69">
         <v>32</v>
       </c>
-      <c r="X19" s="69">
+      <c r="X19" s="73">
         <v>11</v>
       </c>
-      <c r="Y19" s="69"/>
-      <c r="Z19" s="69"/>
-      <c r="AA19" s="69"/>
-      <c r="AB19" s="69"/>
-      <c r="AC19" s="69" t="s">
+      <c r="Y19" s="73"/>
+      <c r="Z19" s="73"/>
+      <c r="AA19" s="73"/>
+      <c r="AB19" s="73"/>
+      <c r="AC19" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="AD19" s="69" t="s">
+      <c r="AD19" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AE19" s="69" t="s">
+      <c r="AE19" s="73" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="18" t="s">
         <v>60</v>
       </c>
@@ -5745,25 +5764,25 @@
       <c r="R20" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="62"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="62"/>
-      <c r="AD20" s="62"/>
-      <c r="AE20" s="62"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
+      <c r="U20" s="66"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="66"/>
+      <c r="X20" s="66"/>
+      <c r="Y20" s="66"/>
+      <c r="Z20" s="66"/>
+      <c r="AA20" s="66"/>
+      <c r="AB20" s="66"/>
+      <c r="AC20" s="66"/>
+      <c r="AD20" s="66"/>
+      <c r="AE20" s="66"/>
     </row>
     <row r="21" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="61">
+      <c r="A21" s="65">
         <v>5</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="67" t="s">
         <v>137</v>
       </c>
       <c r="C21" s="38" t="s">
@@ -5814,39 +5833,39 @@
       <c r="R21" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S21" s="65">
+      <c r="S21" s="69">
         <v>19</v>
       </c>
-      <c r="T21" s="65">
+      <c r="T21" s="69">
         <v>188</v>
       </c>
-      <c r="U21" s="65"/>
-      <c r="V21" s="65">
+      <c r="U21" s="69"/>
+      <c r="V21" s="69">
         <v>62</v>
       </c>
-      <c r="W21" s="65">
+      <c r="W21" s="69">
         <v>32</v>
       </c>
-      <c r="X21" s="69">
+      <c r="X21" s="73">
         <v>12</v>
       </c>
-      <c r="Y21" s="69"/>
-      <c r="Z21" s="69"/>
-      <c r="AA21" s="69"/>
-      <c r="AB21" s="69"/>
-      <c r="AC21" s="69" t="s">
+      <c r="Y21" s="73"/>
+      <c r="Z21" s="73"/>
+      <c r="AA21" s="73"/>
+      <c r="AB21" s="73"/>
+      <c r="AC21" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="AD21" s="69" t="s">
+      <c r="AD21" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AE21" s="69" t="s">
+      <c r="AE21" s="73" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
-      <c r="B22" s="62"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="18" t="s">
         <v>60</v>
       </c>
@@ -5895,25 +5914,25 @@
       <c r="R22" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="S22" s="62"/>
-      <c r="T22" s="62"/>
-      <c r="U22" s="62"/>
-      <c r="V22" s="62"/>
-      <c r="W22" s="62"/>
-      <c r="X22" s="62"/>
-      <c r="Y22" s="62"/>
-      <c r="Z22" s="62"/>
-      <c r="AA22" s="62"/>
-      <c r="AB22" s="62"/>
-      <c r="AC22" s="62"/>
-      <c r="AD22" s="62"/>
-      <c r="AE22" s="62"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+      <c r="Z22" s="66"/>
+      <c r="AA22" s="66"/>
+      <c r="AB22" s="66"/>
+      <c r="AC22" s="66"/>
+      <c r="AD22" s="66"/>
+      <c r="AE22" s="66"/>
     </row>
     <row r="23" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="61">
+      <c r="A23" s="65">
         <v>6</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="67" t="s">
         <v>138</v>
       </c>
       <c r="C23" s="38" t="s">
@@ -5964,41 +5983,41 @@
       <c r="R23" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S23" s="65">
+      <c r="S23" s="69">
         <v>18</v>
       </c>
-      <c r="T23" s="65">
+      <c r="T23" s="69">
         <v>168</v>
       </c>
-      <c r="U23" s="65"/>
-      <c r="V23" s="65">
+      <c r="U23" s="69"/>
+      <c r="V23" s="69">
         <v>64</v>
       </c>
-      <c r="W23" s="69">
+      <c r="W23" s="73">
         <v>4</v>
       </c>
-      <c r="X23" s="69">
+      <c r="X23" s="73">
         <v>12</v>
       </c>
-      <c r="Y23" s="69"/>
-      <c r="Z23" s="69">
+      <c r="Y23" s="73"/>
+      <c r="Z23" s="73">
         <v>1</v>
       </c>
-      <c r="AA23" s="69"/>
-      <c r="AB23" s="69"/>
-      <c r="AC23" s="69" t="s">
+      <c r="AA23" s="73"/>
+      <c r="AB23" s="73"/>
+      <c r="AC23" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="AD23" s="69" t="s">
+      <c r="AD23" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="AE23" s="69" t="s">
+      <c r="AE23" s="73" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="62"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="17" t="s">
         <v>58</v>
       </c>
@@ -6047,25 +6066,25 @@
       <c r="R24" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="62"/>
-      <c r="Y24" s="62"/>
-      <c r="Z24" s="62"/>
-      <c r="AA24" s="62"/>
-      <c r="AB24" s="62"/>
-      <c r="AC24" s="62"/>
-      <c r="AD24" s="62"/>
-      <c r="AE24" s="62"/>
+      <c r="S24" s="66"/>
+      <c r="T24" s="66"/>
+      <c r="U24" s="66"/>
+      <c r="V24" s="66"/>
+      <c r="W24" s="66"/>
+      <c r="X24" s="66"/>
+      <c r="Y24" s="66"/>
+      <c r="Z24" s="66"/>
+      <c r="AA24" s="66"/>
+      <c r="AB24" s="66"/>
+      <c r="AC24" s="66"/>
+      <c r="AD24" s="66"/>
+      <c r="AE24" s="66"/>
     </row>
     <row r="25" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="61">
+      <c r="A25" s="65">
         <v>7</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="67" t="s">
         <v>140</v>
       </c>
       <c r="C25" s="17" t="s">
@@ -6116,39 +6135,39 @@
       <c r="R25" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S25" s="65">
+      <c r="S25" s="69">
         <v>20</v>
       </c>
-      <c r="T25" s="65">
+      <c r="T25" s="69">
         <v>192</v>
       </c>
-      <c r="U25" s="65"/>
-      <c r="V25" s="65">
+      <c r="U25" s="69"/>
+      <c r="V25" s="69">
         <v>64</v>
       </c>
-      <c r="W25" s="65">
+      <c r="W25" s="69">
         <v>36</v>
       </c>
-      <c r="X25" s="69">
+      <c r="X25" s="73">
         <v>11</v>
       </c>
-      <c r="Y25" s="69"/>
-      <c r="Z25" s="69"/>
-      <c r="AA25" s="69"/>
-      <c r="AB25" s="69"/>
-      <c r="AC25" s="69" t="s">
+      <c r="Y25" s="73"/>
+      <c r="Z25" s="73"/>
+      <c r="AA25" s="73"/>
+      <c r="AB25" s="73"/>
+      <c r="AC25" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AD25" s="69" t="s">
+      <c r="AD25" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AE25" s="69" t="s">
+      <c r="AE25" s="73" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="62"/>
-      <c r="B26" s="62"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="17" t="s">
         <v>59</v>
       </c>
@@ -6197,25 +6216,25 @@
       <c r="R26" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="S26" s="62"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="62"/>
-      <c r="V26" s="62"/>
-      <c r="W26" s="62"/>
-      <c r="X26" s="62"/>
-      <c r="Y26" s="62"/>
-      <c r="Z26" s="62"/>
-      <c r="AA26" s="62"/>
-      <c r="AB26" s="62"/>
-      <c r="AC26" s="62"/>
-      <c r="AD26" s="62"/>
-      <c r="AE26" s="62"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="66"/>
+      <c r="U26" s="66"/>
+      <c r="V26" s="66"/>
+      <c r="W26" s="66"/>
+      <c r="X26" s="66"/>
+      <c r="Y26" s="66"/>
+      <c r="Z26" s="66"/>
+      <c r="AA26" s="66"/>
+      <c r="AB26" s="66"/>
+      <c r="AC26" s="66"/>
+      <c r="AD26" s="66"/>
+      <c r="AE26" s="66"/>
     </row>
     <row r="27" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61">
+      <c r="A27" s="65">
         <v>8</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="67" t="s">
         <v>141</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -6266,41 +6285,41 @@
       <c r="R27" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S27" s="65">
+      <c r="S27" s="69">
         <v>7</v>
       </c>
-      <c r="T27" s="65">
+      <c r="T27" s="69">
         <v>68</v>
       </c>
-      <c r="U27" s="65"/>
-      <c r="V27" s="65">
+      <c r="U27" s="69"/>
+      <c r="V27" s="69">
         <v>16</v>
       </c>
-      <c r="W27" s="69">
+      <c r="W27" s="73">
         <v>8</v>
       </c>
-      <c r="X27" s="69">
+      <c r="X27" s="73">
         <v>3</v>
       </c>
-      <c r="Y27" s="69">
+      <c r="Y27" s="73">
         <v>21</v>
       </c>
-      <c r="Z27" s="69"/>
-      <c r="AA27" s="69"/>
-      <c r="AB27" s="69"/>
-      <c r="AC27" s="69" t="s">
+      <c r="Z27" s="73"/>
+      <c r="AA27" s="73"/>
+      <c r="AB27" s="73"/>
+      <c r="AC27" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="AD27" s="69" t="s">
+      <c r="AD27" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="AE27" s="69" t="s">
+      <c r="AE27" s="73" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="62"/>
-      <c r="B28" s="62"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="66"/>
       <c r="C28" s="17" t="s">
         <v>67</v>
       </c>
@@ -6349,25 +6368,25 @@
       <c r="R28" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="S28" s="62"/>
-      <c r="T28" s="62"/>
-      <c r="U28" s="62"/>
-      <c r="V28" s="62"/>
-      <c r="W28" s="62"/>
-      <c r="X28" s="62"/>
-      <c r="Y28" s="62"/>
-      <c r="Z28" s="62"/>
-      <c r="AA28" s="62"/>
-      <c r="AB28" s="62"/>
-      <c r="AC28" s="62"/>
-      <c r="AD28" s="62"/>
-      <c r="AE28" s="62"/>
+      <c r="S28" s="66"/>
+      <c r="T28" s="66"/>
+      <c r="U28" s="66"/>
+      <c r="V28" s="66"/>
+      <c r="W28" s="66"/>
+      <c r="X28" s="66"/>
+      <c r="Y28" s="66"/>
+      <c r="Z28" s="66"/>
+      <c r="AA28" s="66"/>
+      <c r="AB28" s="66"/>
+      <c r="AC28" s="66"/>
+      <c r="AD28" s="66"/>
+      <c r="AE28" s="66"/>
     </row>
     <row r="29" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="61">
+      <c r="A29" s="65">
         <v>9</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="67" t="s">
         <v>142</v>
       </c>
       <c r="C29" s="17" t="s">
@@ -6418,41 +6437,41 @@
       <c r="R29" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S29" s="90">
+      <c r="S29" s="94">
         <v>5</v>
       </c>
-      <c r="T29" s="90">
+      <c r="T29" s="94">
         <v>48</v>
       </c>
-      <c r="U29" s="90"/>
-      <c r="V29" s="90">
+      <c r="U29" s="94"/>
+      <c r="V29" s="94">
         <v>16</v>
       </c>
-      <c r="W29" s="90"/>
-      <c r="X29" s="88">
+      <c r="W29" s="94"/>
+      <c r="X29" s="92">
         <v>4</v>
       </c>
-      <c r="Y29" s="88">
+      <c r="Y29" s="92">
         <v>13</v>
       </c>
-      <c r="Z29" s="69">
+      <c r="Z29" s="73">
         <v>9</v>
       </c>
-      <c r="AA29" s="69"/>
-      <c r="AB29" s="69"/>
-      <c r="AC29" s="69" t="s">
+      <c r="AA29" s="73"/>
+      <c r="AB29" s="73"/>
+      <c r="AC29" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="AD29" s="69" t="s">
+      <c r="AD29" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="AE29" s="69" t="s">
+      <c r="AE29" s="73" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="62"/>
-      <c r="B30" s="62"/>
+      <c r="A30" s="66"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="17" t="s">
         <v>67</v>
       </c>
@@ -6501,25 +6520,25 @@
       <c r="R30" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="S30" s="62"/>
-      <c r="T30" s="62"/>
-      <c r="U30" s="62"/>
-      <c r="V30" s="62"/>
-      <c r="W30" s="62"/>
-      <c r="X30" s="62"/>
-      <c r="Y30" s="62"/>
-      <c r="Z30" s="62"/>
-      <c r="AA30" s="62"/>
-      <c r="AB30" s="62"/>
-      <c r="AC30" s="62"/>
-      <c r="AD30" s="62"/>
-      <c r="AE30" s="62"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
+      <c r="V30" s="66"/>
+      <c r="W30" s="66"/>
+      <c r="X30" s="66"/>
+      <c r="Y30" s="66"/>
+      <c r="Z30" s="66"/>
+      <c r="AA30" s="66"/>
+      <c r="AB30" s="66"/>
+      <c r="AC30" s="66"/>
+      <c r="AD30" s="66"/>
+      <c r="AE30" s="66"/>
     </row>
     <row r="31" spans="1:31" s="15" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="72">
+      <c r="A31" s="76">
         <v>10</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="67" t="s">
         <v>144</v>
       </c>
       <c r="C31" s="17" t="s">
@@ -6570,39 +6589,39 @@
       <c r="R31" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S31" s="65">
+      <c r="S31" s="69">
         <v>14</v>
       </c>
-      <c r="T31" s="65">
+      <c r="T31" s="69">
         <v>128</v>
       </c>
-      <c r="U31" s="65"/>
-      <c r="V31" s="65">
+      <c r="U31" s="69"/>
+      <c r="V31" s="69">
         <v>10</v>
       </c>
-      <c r="W31" s="69"/>
-      <c r="X31" s="69">
+      <c r="W31" s="73"/>
+      <c r="X31" s="73">
         <v>11</v>
       </c>
-      <c r="Y31" s="69">
+      <c r="Y31" s="73">
         <v>6</v>
       </c>
-      <c r="Z31" s="69"/>
-      <c r="AA31" s="69"/>
-      <c r="AB31" s="69"/>
-      <c r="AC31" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD31" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE31" s="69" t="s">
+      <c r="Z31" s="73"/>
+      <c r="AA31" s="73"/>
+      <c r="AB31" s="73"/>
+      <c r="AC31" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD31" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE31" s="73" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:31" s="15" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="62"/>
-      <c r="B32" s="62"/>
+      <c r="A32" s="66"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="17" t="s">
         <v>25</v>
       </c>
@@ -6651,25 +6670,25 @@
       <c r="R32" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="S32" s="62"/>
-      <c r="T32" s="62"/>
-      <c r="U32" s="62"/>
-      <c r="V32" s="62"/>
-      <c r="W32" s="62"/>
-      <c r="X32" s="62"/>
-      <c r="Y32" s="62"/>
-      <c r="Z32" s="62"/>
-      <c r="AA32" s="62"/>
-      <c r="AB32" s="62"/>
-      <c r="AC32" s="62"/>
-      <c r="AD32" s="62"/>
-      <c r="AE32" s="62"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="66"/>
+      <c r="U32" s="66"/>
+      <c r="V32" s="66"/>
+      <c r="W32" s="66"/>
+      <c r="X32" s="66"/>
+      <c r="Y32" s="66"/>
+      <c r="Z32" s="66"/>
+      <c r="AA32" s="66"/>
+      <c r="AB32" s="66"/>
+      <c r="AC32" s="66"/>
+      <c r="AD32" s="66"/>
+      <c r="AE32" s="66"/>
     </row>
     <row r="33" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="61">
+      <c r="A33" s="65">
         <v>11</v>
       </c>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="67" t="s">
         <v>145</v>
       </c>
       <c r="C33" s="17" t="s">
@@ -6720,37 +6739,37 @@
       <c r="R33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S33" s="65">
+      <c r="S33" s="69">
         <v>15</v>
       </c>
-      <c r="T33" s="65">
+      <c r="T33" s="69">
         <v>144</v>
       </c>
-      <c r="U33" s="65"/>
-      <c r="V33" s="65">
+      <c r="U33" s="69"/>
+      <c r="V33" s="69">
         <v>48</v>
       </c>
-      <c r="W33" s="69"/>
-      <c r="X33" s="69">
+      <c r="W33" s="73"/>
+      <c r="X33" s="73">
         <v>10</v>
       </c>
-      <c r="Y33" s="69"/>
-      <c r="Z33" s="69"/>
-      <c r="AA33" s="69"/>
-      <c r="AB33" s="69"/>
-      <c r="AC33" s="69" t="s">
+      <c r="Y33" s="73"/>
+      <c r="Z33" s="73"/>
+      <c r="AA33" s="73"/>
+      <c r="AB33" s="73"/>
+      <c r="AC33" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="AD33" s="69" t="s">
+      <c r="AD33" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="AE33" s="69" t="s">
+      <c r="AE33" s="73" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="62"/>
-      <c r="B34" s="62"/>
+      <c r="A34" s="66"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="20" t="s">
         <v>81</v>
       </c>
@@ -6787,25 +6806,25 @@
       <c r="P34" s="17"/>
       <c r="Q34" s="20"/>
       <c r="R34" s="17"/>
-      <c r="S34" s="62"/>
-      <c r="T34" s="62"/>
-      <c r="U34" s="62"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="62"/>
-      <c r="X34" s="62"/>
-      <c r="Y34" s="62"/>
-      <c r="Z34" s="62"/>
-      <c r="AA34" s="62"/>
-      <c r="AB34" s="62"/>
-      <c r="AC34" s="62"/>
-      <c r="AD34" s="62"/>
-      <c r="AE34" s="62"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="66"/>
+      <c r="U34" s="66"/>
+      <c r="V34" s="66"/>
+      <c r="W34" s="66"/>
+      <c r="X34" s="66"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="66"/>
+      <c r="AA34" s="66"/>
+      <c r="AB34" s="66"/>
+      <c r="AC34" s="66"/>
+      <c r="AD34" s="66"/>
+      <c r="AE34" s="66"/>
     </row>
     <row r="35" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="61">
+      <c r="A35" s="65">
         <v>12</v>
       </c>
-      <c r="B35" s="95" t="s">
+      <c r="B35" s="99" t="s">
         <v>146</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -6856,33 +6875,33 @@
       <c r="R35" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S35" s="65">
+      <c r="S35" s="69">
         <v>6</v>
       </c>
-      <c r="T35" s="69">
+      <c r="T35" s="73">
         <v>33.599999999999987</v>
       </c>
-      <c r="U35" s="65"/>
-      <c r="V35" s="65"/>
-      <c r="W35" s="65">
+      <c r="U35" s="69"/>
+      <c r="V35" s="69"/>
+      <c r="W35" s="69">
         <v>5.6</v>
       </c>
-      <c r="X35" s="69">
+      <c r="X35" s="73">
         <v>9</v>
       </c>
-      <c r="Y35" s="69">
+      <c r="Y35" s="73">
         <v>16</v>
       </c>
-      <c r="Z35" s="69"/>
+      <c r="Z35" s="73"/>
       <c r="AA35" s="44"/>
-      <c r="AB35" s="97"/>
-      <c r="AC35" s="69"/>
-      <c r="AD35" s="69"/>
-      <c r="AE35" s="69"/>
+      <c r="AB35" s="101"/>
+      <c r="AC35" s="73"/>
+      <c r="AD35" s="73"/>
+      <c r="AE35" s="73"/>
     </row>
     <row r="36" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="62"/>
-      <c r="B36" s="96"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="17" t="s">
         <v>67</v>
       </c>
@@ -6931,25 +6950,25 @@
       <c r="R36" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="S36" s="62"/>
-      <c r="T36" s="62"/>
-      <c r="U36" s="62"/>
-      <c r="V36" s="62"/>
-      <c r="W36" s="62"/>
-      <c r="X36" s="62"/>
-      <c r="Y36" s="62"/>
-      <c r="Z36" s="62"/>
+      <c r="S36" s="66"/>
+      <c r="T36" s="66"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="66"/>
+      <c r="W36" s="66"/>
+      <c r="X36" s="66"/>
+      <c r="Y36" s="66"/>
+      <c r="Z36" s="66"/>
       <c r="AA36" s="45"/>
-      <c r="AB36" s="56"/>
-      <c r="AC36" s="62"/>
-      <c r="AD36" s="62"/>
-      <c r="AE36" s="62"/>
+      <c r="AB36" s="60"/>
+      <c r="AC36" s="66"/>
+      <c r="AD36" s="66"/>
+      <c r="AE36" s="66"/>
     </row>
     <row r="37" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="61">
+      <c r="A37" s="65">
         <v>13</v>
       </c>
-      <c r="B37" s="95" t="s">
+      <c r="B37" s="99" t="s">
         <v>148</v>
       </c>
       <c r="C37" s="17" t="s">
@@ -7000,31 +7019,31 @@
       <c r="R37" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S37" s="65">
+      <c r="S37" s="69">
         <v>18</v>
       </c>
-      <c r="T37" s="69">
+      <c r="T37" s="73">
         <v>100.8</v>
       </c>
-      <c r="U37" s="65"/>
-      <c r="V37" s="65"/>
-      <c r="W37" s="65">
+      <c r="U37" s="69"/>
+      <c r="V37" s="69"/>
+      <c r="W37" s="69">
         <v>11.2</v>
       </c>
-      <c r="X37" s="69">
+      <c r="X37" s="73">
         <v>13</v>
       </c>
-      <c r="Y37" s="69"/>
-      <c r="Z37" s="69"/>
+      <c r="Y37" s="73"/>
+      <c r="Z37" s="73"/>
       <c r="AA37" s="44"/>
-      <c r="AB37" s="97"/>
-      <c r="AC37" s="69"/>
-      <c r="AD37" s="69"/>
-      <c r="AE37" s="69"/>
+      <c r="AB37" s="101"/>
+      <c r="AC37" s="73"/>
+      <c r="AD37" s="73"/>
+      <c r="AE37" s="73"/>
     </row>
     <row r="38" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="62"/>
-      <c r="B38" s="96"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="17" t="s">
         <v>147</v>
       </c>
@@ -7073,25 +7092,25 @@
       <c r="R38" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="S38" s="62"/>
-      <c r="T38" s="62"/>
-      <c r="U38" s="62"/>
-      <c r="V38" s="62"/>
-      <c r="W38" s="62"/>
-      <c r="X38" s="62"/>
-      <c r="Y38" s="62"/>
-      <c r="Z38" s="62"/>
+      <c r="S38" s="66"/>
+      <c r="T38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="66"/>
+      <c r="Y38" s="66"/>
+      <c r="Z38" s="66"/>
       <c r="AA38" s="45"/>
-      <c r="AB38" s="56"/>
-      <c r="AC38" s="62"/>
-      <c r="AD38" s="62"/>
-      <c r="AE38" s="62"/>
+      <c r="AB38" s="60"/>
+      <c r="AC38" s="66"/>
+      <c r="AD38" s="66"/>
+      <c r="AE38" s="66"/>
     </row>
     <row r="39" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="61">
+      <c r="A39" s="65">
         <v>14</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="102" t="s">
         <v>149</v>
       </c>
       <c r="C39" s="17" t="s">
@@ -7142,31 +7161,31 @@
       <c r="R39" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S39" s="65">
+      <c r="S39" s="69">
         <v>18</v>
       </c>
-      <c r="T39" s="69">
+      <c r="T39" s="73">
         <v>144</v>
       </c>
-      <c r="U39" s="65"/>
-      <c r="V39" s="65"/>
-      <c r="W39" s="65">
+      <c r="U39" s="69"/>
+      <c r="V39" s="69"/>
+      <c r="W39" s="69">
         <v>16</v>
       </c>
-      <c r="X39" s="69">
+      <c r="X39" s="73">
         <v>13</v>
       </c>
-      <c r="Y39" s="69"/>
-      <c r="Z39" s="69"/>
-      <c r="AA39" s="69"/>
-      <c r="AB39" s="69"/>
-      <c r="AC39" s="69"/>
-      <c r="AD39" s="69"/>
-      <c r="AE39" s="69"/>
+      <c r="Y39" s="73"/>
+      <c r="Z39" s="73"/>
+      <c r="AA39" s="73"/>
+      <c r="AB39" s="73"/>
+      <c r="AC39" s="73"/>
+      <c r="AD39" s="73"/>
+      <c r="AE39" s="73"/>
     </row>
     <row r="40" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="62"/>
-      <c r="B40" s="54"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="17" t="s">
         <v>25</v>
       </c>
@@ -7215,25 +7234,25 @@
       <c r="R40" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S40" s="62"/>
-      <c r="T40" s="62"/>
-      <c r="U40" s="62"/>
-      <c r="V40" s="62"/>
-      <c r="W40" s="62"/>
-      <c r="X40" s="62"/>
-      <c r="Y40" s="62"/>
-      <c r="Z40" s="62"/>
-      <c r="AA40" s="62"/>
-      <c r="AB40" s="62"/>
-      <c r="AC40" s="62"/>
-      <c r="AD40" s="62"/>
-      <c r="AE40" s="62"/>
+      <c r="S40" s="66"/>
+      <c r="T40" s="66"/>
+      <c r="U40" s="66"/>
+      <c r="V40" s="66"/>
+      <c r="W40" s="66"/>
+      <c r="X40" s="66"/>
+      <c r="Y40" s="66"/>
+      <c r="Z40" s="66"/>
+      <c r="AA40" s="66"/>
+      <c r="AB40" s="66"/>
+      <c r="AC40" s="66"/>
+      <c r="AD40" s="66"/>
+      <c r="AE40" s="66"/>
     </row>
     <row r="41" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="61">
+      <c r="A41" s="65">
         <v>15</v>
       </c>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="102" t="s">
         <v>150</v>
       </c>
       <c r="C41" s="17" t="s">
@@ -7284,33 +7303,33 @@
       <c r="R41" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S41" s="65">
+      <c r="S41" s="69">
         <v>17</v>
       </c>
-      <c r="T41" s="69">
+      <c r="T41" s="73">
         <v>136</v>
       </c>
-      <c r="U41" s="65"/>
-      <c r="V41" s="65"/>
-      <c r="W41" s="65">
+      <c r="U41" s="69"/>
+      <c r="V41" s="69"/>
+      <c r="W41" s="69">
         <v>16</v>
       </c>
-      <c r="X41" s="69">
+      <c r="X41" s="73">
         <v>13</v>
       </c>
-      <c r="Y41" s="69"/>
-      <c r="Z41" s="69"/>
-      <c r="AA41" s="69">
+      <c r="Y41" s="73"/>
+      <c r="Z41" s="73"/>
+      <c r="AA41" s="73">
         <v>1</v>
       </c>
-      <c r="AB41" s="69"/>
-      <c r="AC41" s="69"/>
-      <c r="AD41" s="69"/>
-      <c r="AE41" s="69"/>
+      <c r="AB41" s="73"/>
+      <c r="AC41" s="73"/>
+      <c r="AD41" s="73"/>
+      <c r="AE41" s="73"/>
     </row>
     <row r="42" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="62"/>
-      <c r="B42" s="54"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="17" t="s">
         <v>25</v>
       </c>
@@ -7359,25 +7378,25 @@
       <c r="R42" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S42" s="62"/>
-      <c r="T42" s="62"/>
-      <c r="U42" s="62"/>
-      <c r="V42" s="62"/>
-      <c r="W42" s="62"/>
-      <c r="X42" s="62"/>
-      <c r="Y42" s="62"/>
-      <c r="Z42" s="62"/>
-      <c r="AA42" s="62"/>
-      <c r="AB42" s="62"/>
-      <c r="AC42" s="62"/>
-      <c r="AD42" s="62"/>
-      <c r="AE42" s="62"/>
+      <c r="S42" s="66"/>
+      <c r="T42" s="66"/>
+      <c r="U42" s="66"/>
+      <c r="V42" s="66"/>
+      <c r="W42" s="66"/>
+      <c r="X42" s="66"/>
+      <c r="Y42" s="66"/>
+      <c r="Z42" s="66"/>
+      <c r="AA42" s="66"/>
+      <c r="AB42" s="66"/>
+      <c r="AC42" s="66"/>
+      <c r="AD42" s="66"/>
+      <c r="AE42" s="66"/>
     </row>
     <row r="43" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="61">
+      <c r="A43" s="65">
         <v>16</v>
       </c>
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="102" t="s">
         <v>152</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -7428,31 +7447,31 @@
       <c r="R43" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="S43" s="65">
+      <c r="S43" s="69">
         <v>18</v>
       </c>
-      <c r="T43" s="69">
+      <c r="T43" s="73">
         <v>144</v>
       </c>
-      <c r="U43" s="65"/>
-      <c r="V43" s="65"/>
-      <c r="W43" s="65">
+      <c r="U43" s="69"/>
+      <c r="V43" s="69"/>
+      <c r="W43" s="69">
         <v>16</v>
       </c>
-      <c r="X43" s="69">
+      <c r="X43" s="73">
         <v>13</v>
       </c>
-      <c r="Y43" s="69"/>
-      <c r="Z43" s="69"/>
-      <c r="AA43" s="69"/>
-      <c r="AB43" s="69"/>
-      <c r="AC43" s="69"/>
-      <c r="AD43" s="69"/>
-      <c r="AE43" s="69"/>
+      <c r="Y43" s="73"/>
+      <c r="Z43" s="73"/>
+      <c r="AA43" s="73"/>
+      <c r="AB43" s="73"/>
+      <c r="AC43" s="73"/>
+      <c r="AD43" s="73"/>
+      <c r="AE43" s="73"/>
     </row>
     <row r="44" spans="1:31" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="62"/>
-      <c r="B44" s="54"/>
+      <c r="A44" s="66"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="17" t="s">
         <v>25</v>
       </c>
@@ -7501,19 +7520,19 @@
       <c r="R44" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="S44" s="62"/>
-      <c r="T44" s="62"/>
-      <c r="U44" s="62"/>
-      <c r="V44" s="62"/>
-      <c r="W44" s="62"/>
-      <c r="X44" s="62"/>
-      <c r="Y44" s="62"/>
-      <c r="Z44" s="62"/>
-      <c r="AA44" s="62"/>
-      <c r="AB44" s="62"/>
-      <c r="AC44" s="62"/>
-      <c r="AD44" s="62"/>
-      <c r="AE44" s="62"/>
+      <c r="S44" s="66"/>
+      <c r="T44" s="66"/>
+      <c r="U44" s="66"/>
+      <c r="V44" s="66"/>
+      <c r="W44" s="66"/>
+      <c r="X44" s="66"/>
+      <c r="Y44" s="66"/>
+      <c r="Z44" s="66"/>
+      <c r="AA44" s="66"/>
+      <c r="AB44" s="66"/>
+      <c r="AC44" s="66"/>
+      <c r="AD44" s="66"/>
+      <c r="AE44" s="66"/>
     </row>
     <row r="45" spans="1:31" ht="5.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
@@ -7549,31 +7568,31 @@
       <c r="AE45" s="12"/>
     </row>
     <row r="46" spans="1:31" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="73" t="s">
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="M46" s="59"/>
-      <c r="N46" s="55"/>
-      <c r="O46" s="55"/>
-      <c r="Q46" s="59" t="s">
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="59"/>
+      <c r="O46" s="59"/>
+      <c r="Q46" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="R46" s="55"/>
-      <c r="S46" s="55"/>
-      <c r="T46" s="55"/>
-      <c r="U46" s="55"/>
+      <c r="R46" s="59"/>
+      <c r="S46" s="59"/>
+      <c r="T46" s="59"/>
+      <c r="U46" s="59"/>
       <c r="V46" s="4"/>
       <c r="W46" s="4" t="s">
         <v>111</v>
@@ -7588,31 +7607,31 @@
       <c r="AE46" s="12"/>
     </row>
     <row r="47" spans="1:31" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="47"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="74" t="s">
+      <c r="A47" s="51"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
-      <c r="K47" s="52"/>
-      <c r="M47" s="60" t="s">
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="M47" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="N47" s="52"/>
-      <c r="O47" s="52"/>
-      <c r="Q47" s="60" t="s">
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="Q47" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="R47" s="52"/>
-      <c r="S47" s="52"/>
-      <c r="T47" s="52"/>
-      <c r="U47" s="52"/>
+      <c r="R47" s="56"/>
+      <c r="S47" s="56"/>
+      <c r="T47" s="56"/>
+      <c r="U47" s="56"/>
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
@@ -7625,31 +7644,31 @@
       <c r="AE47" s="12"/>
     </row>
     <row r="48" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="58" t="s">
+      <c r="A48" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="73" t="s">
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="Q48" s="59" t="s">
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="59"/>
+      <c r="K48" s="59"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="59"/>
+      <c r="O48" s="59"/>
+      <c r="Q48" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="R48" s="55"/>
-      <c r="S48" s="55"/>
-      <c r="T48" s="55"/>
-      <c r="U48" s="55"/>
+      <c r="R48" s="59"/>
+      <c r="S48" s="59"/>
+      <c r="T48" s="59"/>
+      <c r="U48" s="59"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4" t="s">
         <v>111</v>
@@ -7664,31 +7683,31 @@
       <c r="AE48" s="4"/>
     </row>
     <row r="49" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="47"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="74" t="s">
+      <c r="A49" s="51"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="52"/>
-      <c r="M49" s="60" t="s">
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="M49" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="N49" s="52"/>
-      <c r="O49" s="52"/>
-      <c r="Q49" s="60" t="s">
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="Q49" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="R49" s="52"/>
-      <c r="S49" s="52"/>
-      <c r="T49" s="52"/>
-      <c r="U49" s="52"/>
+      <c r="R49" s="56"/>
+      <c r="S49" s="56"/>
+      <c r="T49" s="56"/>
+      <c r="U49" s="56"/>
       <c r="V49" s="4"/>
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
@@ -7701,31 +7720,31 @@
       <c r="AE49" s="4"/>
     </row>
     <row r="50" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="73" t="s">
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="55"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="55"/>
-      <c r="O50" s="55"/>
-      <c r="Q50" s="59" t="s">
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="59"/>
+      <c r="K50" s="59"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="59"/>
+      <c r="O50" s="59"/>
+      <c r="Q50" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="R50" s="55"/>
-      <c r="S50" s="55"/>
-      <c r="T50" s="55"/>
-      <c r="U50" s="55"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="59"/>
+      <c r="T50" s="59"/>
+      <c r="U50" s="59"/>
       <c r="V50" s="4"/>
       <c r="W50" s="4" t="s">
         <v>111</v>
@@ -7740,31 +7759,31 @@
       <c r="AE50" s="4"/>
     </row>
     <row r="51" spans="1:31" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="47"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="77" t="s">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="M51" s="46" t="s">
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="M51" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="N51" s="47"/>
-      <c r="O51" s="47"/>
-      <c r="Q51" s="60" t="s">
+      <c r="N51" s="51"/>
+      <c r="O51" s="51"/>
+      <c r="Q51" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="R51" s="52"/>
-      <c r="S51" s="52"/>
-      <c r="T51" s="52"/>
-      <c r="U51" s="52"/>
+      <c r="R51" s="56"/>
+      <c r="S51" s="56"/>
+      <c r="T51" s="56"/>
+      <c r="U51" s="56"/>
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
       <c r="X51" s="4"/>

</xml_diff>

<commit_message>
refactor logic (prepared_range -> splited_cells)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\report_card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\report_card\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5897" tabRatio="412"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5895" tabRatio="412" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="машинисты" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="170">
   <si>
     <t>ГОСУДАРСТВЕННОЕ УНИТАРНОЕ ПРЕДПРИЯТИЕ НЕНЕЦКОГО АВТОНОМНОГО ОКРУГА "НАРЬЯН-МАРСКАЯ ЭЛЕКТРОСТАНЦИЯ"</t>
   </si>
@@ -533,13 +533,28 @@
   </si>
   <si>
     <t>НОД</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> 20/</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -606,6 +621,13 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="7">
@@ -835,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -964,50 +986,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1015,69 +1008,111 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1088,19 +1123,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1407,293 +1433,293 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="S29" sqref="S29:AB36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="14" width="6" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
     <col min="16" max="16" width="6" customWidth="1"/>
-    <col min="17" max="17" width="9.453125" customWidth="1"/>
+    <col min="17" max="17" width="9.5" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
-    <col min="19" max="19" width="5.453125" customWidth="1"/>
-    <col min="20" max="20" width="5.1796875" customWidth="1"/>
-    <col min="21" max="21" width="4.1796875" customWidth="1"/>
-    <col min="22" max="22" width="5.36328125" customWidth="1"/>
-    <col min="23" max="23" width="4.453125" customWidth="1"/>
-    <col min="24" max="24" width="5.1796875" customWidth="1"/>
+    <col min="19" max="19" width="5.5" customWidth="1"/>
+    <col min="20" max="20" width="5.1640625" customWidth="1"/>
+    <col min="21" max="21" width="4.1640625" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" customWidth="1"/>
+    <col min="23" max="23" width="4.5" customWidth="1"/>
+    <col min="24" max="24" width="5.1640625" customWidth="1"/>
     <col min="25" max="25" width="4" customWidth="1"/>
-    <col min="26" max="26" width="6.453125" customWidth="1"/>
-    <col min="27" max="27" width="6.36328125" customWidth="1"/>
+    <col min="26" max="26" width="6.5" customWidth="1"/>
+    <col min="27" max="27" width="6.33203125" customWidth="1"/>
     <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="6.6328125" customWidth="1"/>
-    <col min="30" max="30" width="7.36328125" customWidth="1"/>
+    <col min="29" max="29" width="6.6640625" customWidth="1"/>
+    <col min="30" max="30" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2" spans="1:40" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:40" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-    </row>
-    <row r="3" spans="1:40" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+    </row>
+    <row r="3" spans="1:40" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-    </row>
-    <row r="4" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57"/>
+    </row>
+    <row r="4" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-    </row>
-    <row r="5" spans="1:40" s="4" customFormat="1" ht="7.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+    </row>
+    <row r="5" spans="1:40" s="4" customFormat="1" ht="7.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q5" s="8"/>
-      <c r="R5" s="57" t="s">
+      <c r="R5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="58"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="82" t="s">
+      <c r="S5" s="54"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="58"/>
-      <c r="W5" s="59"/>
-      <c r="Z5" s="49" t="s">
+      <c r="V5" s="54"/>
+      <c r="W5" s="71"/>
+      <c r="Z5" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="51"/>
+      <c r="AA5" s="75"/>
+      <c r="AB5" s="75"/>
+      <c r="AC5" s="90"/>
       <c r="AD5" s="28"/>
       <c r="AE5" s="28"/>
       <c r="AF5" s="28"/>
       <c r="AM5" s="28"/>
       <c r="AN5" s="28"/>
     </row>
-    <row r="6" spans="1:40" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q6" s="8"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="61"/>
-      <c r="W6" s="62"/>
-      <c r="Z6" s="49" t="s">
+      <c r="R6" s="77"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="78"/>
+      <c r="Z6" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="AA6" s="51"/>
-      <c r="AB6" s="79" t="s">
+      <c r="AA6" s="90"/>
+      <c r="AB6" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="AC6" s="59"/>
+      <c r="AC6" s="71"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:40" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K7" s="83" t="s">
+    <row r="7" spans="1:40" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="63">
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="72">
         <v>5</v>
       </c>
-      <c r="S7" s="55"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="71">
+      <c r="S7" s="67"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="88">
         <v>44712</v>
       </c>
-      <c r="V7" s="55"/>
-      <c r="W7" s="56"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="68"/>
       <c r="X7" s="28"/>
       <c r="Y7" s="28"/>
-      <c r="Z7" s="49" t="s">
+      <c r="Z7" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="63" t="s">
+      <c r="AA7" s="90"/>
+      <c r="AB7" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="56"/>
-    </row>
-    <row r="8" spans="1:40" s="28" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="83" t="s">
+      <c r="AC7" s="68"/>
+    </row>
+    <row r="8" spans="1:40" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87"/>
-      <c r="R8" s="87"/>
-    </row>
-    <row r="9" spans="1:40" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="s">
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+    </row>
+    <row r="9" spans="1:40" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="85" t="s">
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="54" t="s">
+      <c r="T9" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="54" t="s">
+      <c r="U9" s="67"/>
+      <c r="V9" s="67"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="56"/>
-      <c r="AB9" s="54" t="s">
+      <c r="Y9" s="67"/>
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="AC9" s="59"/>
-    </row>
-    <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
+      <c r="AC9" s="71"/>
+    </row>
+    <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="32" t="s">
         <v>20</v>
       </c>
@@ -1742,37 +1768,37 @@
       <c r="R10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="S10" s="48"/>
-      <c r="T10" s="88" t="s">
+      <c r="S10" s="59"/>
+      <c r="T10" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="88" t="s">
+      <c r="U10" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="88" t="s">
+      <c r="V10" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="86" t="s">
+      <c r="W10" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="X10" s="81" t="s">
+      <c r="X10" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="Y10" s="81" t="s">
+      <c r="Y10" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="Z10" s="81" t="s">
+      <c r="Z10" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="AA10" s="81" t="s">
+      <c r="AA10" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="62"/>
-    </row>
-    <row r="11" spans="1:40" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
+      <c r="AB10" s="77"/>
+      <c r="AC10" s="78"/>
+    </row>
+    <row r="11" spans="1:40" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="30" t="s">
         <v>41</v>
       </c>
@@ -1821,11 +1847,11 @@
       <c r="R11" s="30">
         <v>31</v>
       </c>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
       <c r="X11" s="45"/>
       <c r="Y11" s="45"/>
       <c r="Z11" s="45"/>
@@ -1840,31 +1866,31 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="69">
+      <c r="C12" s="87">
         <v>3</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="71"/>
       <c r="S12" s="43">
         <v>4</v>
       </c>
@@ -1902,11 +1928,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67">
+    <row r="13" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="50">
         <v>1</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="51" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -1957,24 +1983,24 @@
       <c r="R13" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S13" s="70"/>
-      <c r="T13" s="77"/>
-      <c r="U13" s="77"/>
-      <c r="V13" s="77"/>
-      <c r="W13" s="47"/>
-      <c r="X13" s="47"/>
-      <c r="Y13" s="47"/>
-      <c r="Z13" s="47"/>
-      <c r="AA13" s="47"/>
-      <c r="AB13" s="47"/>
-      <c r="AC13" s="47" t="s">
+      <c r="S13" s="44"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58" t="s">
         <v>53</v>
       </c>
       <c r="AD13" s="46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="45"/>
       <c r="B14" s="45"/>
       <c r="C14" s="19" t="s">
@@ -2026,23 +2052,23 @@
         <v>66</v>
       </c>
       <c r="S14" s="45"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="48"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="48"/>
-      <c r="AB14" s="48"/>
-      <c r="AC14" s="48"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="59"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="59"/>
+      <c r="AC14" s="59"/>
       <c r="AD14" s="45"/>
     </row>
-    <row r="15" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67">
+    <row r="15" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="51" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -2093,10 +2119,10 @@
       <c r="R15" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="70"/>
-      <c r="V15" s="70"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
       <c r="W15" s="46"/>
       <c r="X15" s="46"/>
       <c r="Y15" s="46"/>
@@ -2110,7 +2136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="19" t="s">
@@ -2174,11 +2200,11 @@
       <c r="AC16" s="45"/>
       <c r="AD16" s="45"/>
     </row>
-    <row r="17" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="67">
+    <row r="17" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="50">
         <v>3</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="51" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="19" t="s">
@@ -2229,24 +2255,24 @@
       <c r="R17" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="S17" s="73"/>
-      <c r="T17" s="73"/>
-      <c r="U17" s="73"/>
-      <c r="V17" s="73"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
-      <c r="Z17" s="44"/>
-      <c r="AA17" s="44"/>
-      <c r="AB17" s="44"/>
-      <c r="AC17" s="44" t="s">
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="52"/>
+      <c r="X17" s="52"/>
+      <c r="Y17" s="52"/>
+      <c r="Z17" s="52"/>
+      <c r="AA17" s="52"/>
+      <c r="AB17" s="52"/>
+      <c r="AC17" s="52" t="s">
         <v>70</v>
       </c>
       <c r="AD17" s="46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="19" t="s">
@@ -2310,11 +2336,11 @@
       <c r="AC18" s="45"/>
       <c r="AD18" s="45"/>
     </row>
-    <row r="19" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67">
+    <row r="19" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="50">
         <v>4</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="51" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2365,10 +2391,10 @@
       <c r="R19" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="44"/>
       <c r="W19" s="46"/>
       <c r="X19" s="46"/>
       <c r="Y19" s="46"/>
@@ -2382,7 +2408,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45"/>
       <c r="B20" s="45"/>
       <c r="C20" s="33" t="s">
@@ -2446,11 +2472,11 @@
       <c r="AC20" s="45"/>
       <c r="AD20" s="45"/>
     </row>
-    <row r="21" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="67">
+    <row r="21" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="50">
         <v>5</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="51" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -2501,24 +2527,24 @@
       <c r="R21" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S21" s="70"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="77"/>
-      <c r="V21" s="77"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
-      <c r="AA21" s="47"/>
-      <c r="AB21" s="47"/>
-      <c r="AC21" s="47" t="s">
+      <c r="S21" s="44"/>
+      <c r="T21" s="63"/>
+      <c r="U21" s="63"/>
+      <c r="V21" s="63"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58" t="s">
         <v>49</v>
       </c>
       <c r="AD21" s="46" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="45"/>
       <c r="B22" s="45"/>
       <c r="C22" s="19" t="s">
@@ -2570,23 +2596,23 @@
         <v>59</v>
       </c>
       <c r="S22" s="45"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="48"/>
-      <c r="W22" s="48"/>
-      <c r="X22" s="48"/>
-      <c r="Y22" s="48"/>
-      <c r="Z22" s="48"/>
-      <c r="AA22" s="48"/>
-      <c r="AB22" s="48"/>
-      <c r="AC22" s="48"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="59"/>
+      <c r="V22" s="59"/>
+      <c r="W22" s="59"/>
+      <c r="X22" s="59"/>
+      <c r="Y22" s="59"/>
+      <c r="Z22" s="59"/>
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="59"/>
+      <c r="AC22" s="59"/>
       <c r="AD22" s="45"/>
     </row>
-    <row r="23" spans="1:30" s="15" customFormat="1" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="72">
+    <row r="23" spans="1:30" s="15" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="83">
         <v>6</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="51" t="s">
         <v>78</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -2637,10 +2663,10 @@
       <c r="R23" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S23" s="70"/>
-      <c r="T23" s="70"/>
-      <c r="U23" s="70"/>
-      <c r="V23" s="70"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
       <c r="W23" s="46"/>
       <c r="X23" s="46"/>
       <c r="Y23" s="46"/>
@@ -2654,7 +2680,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="15" customFormat="1" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" s="15" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="45"/>
       <c r="B24" s="45"/>
       <c r="C24" s="33" t="s">
@@ -2718,11 +2744,11 @@
       <c r="AC24" s="45"/>
       <c r="AD24" s="45"/>
     </row>
-    <row r="25" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="67">
+    <row r="25" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="50">
         <v>7</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="51" t="s">
         <v>79</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -2773,11 +2799,11 @@
       <c r="R25" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S25" s="70"/>
-      <c r="T25" s="70"/>
-      <c r="U25" s="70"/>
-      <c r="V25" s="70"/>
-      <c r="W25" s="70"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="44"/>
       <c r="X25" s="46"/>
       <c r="Y25" s="46"/>
       <c r="Z25" s="46"/>
@@ -2790,7 +2816,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="45"/>
       <c r="B26" s="45"/>
       <c r="C26" s="19" t="s">
@@ -2854,11 +2880,11 @@
       <c r="AC26" s="45"/>
       <c r="AD26" s="45"/>
     </row>
-    <row r="27" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="67">
+    <row r="27" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="50">
         <v>8</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="51" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2909,11 +2935,11 @@
       <c r="R27" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S27" s="70"/>
-      <c r="T27" s="70"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="70"/>
-      <c r="W27" s="70"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="44"/>
       <c r="X27" s="46"/>
       <c r="Y27" s="46"/>
       <c r="Z27" s="46"/>
@@ -2926,7 +2952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
       <c r="C28" s="20" t="s">
@@ -2990,11 +3016,11 @@
       <c r="AC28" s="45"/>
       <c r="AD28" s="45"/>
     </row>
-    <row r="29" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="67">
+    <row r="29" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="50">
         <v>9</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="51" t="s">
         <v>84</v>
       </c>
       <c r="C29" s="19" t="s">
@@ -3045,24 +3071,24 @@
       <c r="R29" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="S29" s="73"/>
-      <c r="T29" s="73"/>
-      <c r="U29" s="73"/>
-      <c r="V29" s="73"/>
-      <c r="W29" s="44"/>
-      <c r="X29" s="44"/>
-      <c r="Y29" s="44"/>
-      <c r="Z29" s="44"/>
-      <c r="AA29" s="44"/>
-      <c r="AB29" s="44"/>
-      <c r="AC29" s="44" t="s">
+      <c r="S29" s="48"/>
+      <c r="T29" s="48"/>
+      <c r="U29" s="48"/>
+      <c r="V29" s="48"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="52"/>
+      <c r="Z29" s="52"/>
+      <c r="AA29" s="52"/>
+      <c r="AB29" s="52"/>
+      <c r="AC29" s="52" t="s">
         <v>85</v>
       </c>
       <c r="AD29" s="46" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="45"/>
       <c r="B30" s="45"/>
       <c r="C30" s="19" t="s">
@@ -3126,11 +3152,11 @@
       <c r="AC30" s="45"/>
       <c r="AD30" s="45"/>
     </row>
-    <row r="31" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="67">
+    <row r="31" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="50">
         <v>10</v>
       </c>
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="51" t="s">
         <v>87</v>
       </c>
       <c r="C31" s="33" t="s">
@@ -3181,16 +3207,16 @@
       <c r="R31" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="S31" s="90"/>
-      <c r="T31" s="90"/>
-      <c r="U31" s="90"/>
-      <c r="V31" s="90"/>
-      <c r="W31" s="90"/>
-      <c r="X31" s="89"/>
-      <c r="Y31" s="89"/>
-      <c r="Z31" s="89"/>
-      <c r="AA31" s="89"/>
-      <c r="AB31" s="89"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="47"/>
+      <c r="V31" s="47"/>
+      <c r="W31" s="47"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="49"/>
+      <c r="Z31" s="49"/>
+      <c r="AA31" s="49"/>
+      <c r="AB31" s="49"/>
       <c r="AC31" s="46" t="s">
         <v>88</v>
       </c>
@@ -3198,7 +3224,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
       <c r="B32" s="45"/>
       <c r="C32" s="33" t="s">
@@ -3262,11 +3288,11 @@
       <c r="AC32" s="45"/>
       <c r="AD32" s="45"/>
     </row>
-    <row r="33" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67">
+    <row r="33" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="50">
         <v>11</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="51" t="s">
         <v>90</v>
       </c>
       <c r="C33" s="19" t="s">
@@ -3317,24 +3343,24 @@
       <c r="R33" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S33" s="73"/>
-      <c r="T33" s="70"/>
-      <c r="U33" s="70"/>
-      <c r="V33" s="70"/>
-      <c r="W33" s="70"/>
+      <c r="S33" s="48"/>
+      <c r="T33" s="44"/>
+      <c r="U33" s="44"/>
+      <c r="V33" s="44"/>
+      <c r="W33" s="44"/>
       <c r="X33" s="46"/>
       <c r="Y33" s="46"/>
       <c r="Z33" s="46"/>
       <c r="AA33" s="46"/>
       <c r="AB33" s="46"/>
-      <c r="AC33" s="44" t="s">
+      <c r="AC33" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="AD33" s="44" t="s">
+      <c r="AD33" s="52" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
       <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
@@ -3398,11 +3424,11 @@
       <c r="AC34" s="45"/>
       <c r="AD34" s="45"/>
     </row>
-    <row r="35" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="67">
+    <row r="35" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="50">
         <v>12</v>
       </c>
-      <c r="B35" s="68" t="s">
+      <c r="B35" s="51" t="s">
         <v>91</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -3453,11 +3479,11 @@
       <c r="R35" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S35" s="70"/>
+      <c r="S35" s="44"/>
       <c r="T35" s="46"/>
-      <c r="U35" s="70"/>
-      <c r="V35" s="70"/>
-      <c r="W35" s="70"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="44"/>
       <c r="X35" s="46"/>
       <c r="Y35" s="46"/>
       <c r="Z35" s="46"/>
@@ -3466,7 +3492,7 @@
       <c r="AC35" s="46"/>
       <c r="AD35" s="46"/>
     </row>
-    <row r="36" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="45"/>
       <c r="B36" s="45"/>
       <c r="C36" s="33" t="s">
@@ -3530,11 +3556,11 @@
       <c r="AC36" s="45"/>
       <c r="AD36" s="45"/>
     </row>
-    <row r="37" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="67">
+    <row r="37" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="50">
         <v>13</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="51" t="s">
         <v>92</v>
       </c>
       <c r="C37" s="19" t="s">
@@ -3585,15 +3611,15 @@
       <c r="R37" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S37" s="70">
+      <c r="S37" s="44">
         <v>18</v>
       </c>
       <c r="T37" s="46">
         <v>144</v>
       </c>
-      <c r="U37" s="70"/>
-      <c r="V37" s="70"/>
-      <c r="W37" s="70"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="44"/>
       <c r="X37" s="46">
         <v>13</v>
       </c>
@@ -3604,7 +3630,7 @@
       <c r="AC37" s="46"/>
       <c r="AD37" s="46"/>
     </row>
-    <row r="38" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
       <c r="B38" s="45"/>
       <c r="C38" s="19" t="s">
@@ -3668,11 +3694,11 @@
       <c r="AC38" s="45"/>
       <c r="AD38" s="45"/>
     </row>
-    <row r="39" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="67">
+    <row r="39" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="50">
         <v>14</v>
       </c>
-      <c r="B39" s="68" t="s">
+      <c r="B39" s="51" t="s">
         <v>93</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -3723,15 +3749,15 @@
       <c r="R39" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S39" s="70">
+      <c r="S39" s="44">
         <v>18</v>
       </c>
       <c r="T39" s="46">
         <v>144</v>
       </c>
-      <c r="U39" s="70"/>
-      <c r="V39" s="70"/>
-      <c r="W39" s="70"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="44"/>
       <c r="X39" s="46">
         <v>13</v>
       </c>
@@ -3742,7 +3768,7 @@
       <c r="AC39" s="46"/>
       <c r="AD39" s="46"/>
     </row>
-    <row r="40" spans="1:30" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="45"/>
       <c r="B40" s="45"/>
       <c r="C40" s="19" t="s">
@@ -3806,7 +3832,7 @@
       <c r="AC40" s="45"/>
       <c r="AD40" s="45"/>
     </row>
-    <row r="41" spans="1:30" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
@@ -3838,32 +3864,32 @@
       <c r="AC41" s="12"/>
       <c r="AD41" s="12"/>
     </row>
-    <row r="42" spans="1:30" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
+    <row r="42" spans="1:30" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="74" t="s">
+      <c r="B42" s="81"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="M42" s="65"/>
-      <c r="N42" s="61"/>
-      <c r="O42" s="61"/>
-      <c r="Q42" s="65" t="s">
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="Q42" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="R42" s="61"/>
-      <c r="S42" s="61"/>
-      <c r="T42" s="61"/>
-      <c r="U42" s="61"/>
+      <c r="R42" s="57"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
       <c r="V42" s="4"/>
       <c r="W42" s="4" t="s">
         <v>97</v>
@@ -3876,32 +3902,32 @@
       <c r="AC42" s="12"/>
       <c r="AD42" s="12"/>
     </row>
-    <row r="43" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="75" t="s">
+    <row r="43" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="81"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="M43" s="66" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="54"/>
+      <c r="M43" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="Q43" s="66" t="s">
+      <c r="N43" s="54"/>
+      <c r="O43" s="54"/>
+      <c r="Q43" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="R43" s="58"/>
-      <c r="S43" s="58"/>
-      <c r="T43" s="58"/>
-      <c r="U43" s="58"/>
+      <c r="R43" s="54"/>
+      <c r="S43" s="54"/>
+      <c r="T43" s="54"/>
+      <c r="U43" s="54"/>
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
@@ -3912,32 +3938,32 @@
       <c r="AC43" s="12"/>
       <c r="AD43" s="12"/>
     </row>
-    <row r="44" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="64" t="s">
+    <row r="44" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="74" t="s">
+      <c r="B44" s="81"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="M44" s="65"/>
-      <c r="N44" s="61"/>
-      <c r="O44" s="61"/>
-      <c r="Q44" s="65" t="s">
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+      <c r="Q44" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="R44" s="61"/>
-      <c r="S44" s="61"/>
-      <c r="T44" s="61"/>
-      <c r="U44" s="61"/>
+      <c r="R44" s="57"/>
+      <c r="S44" s="57"/>
+      <c r="T44" s="57"/>
+      <c r="U44" s="57"/>
       <c r="V44" s="4"/>
       <c r="W44" s="4" t="s">
         <v>97</v>
@@ -3950,32 +3976,32 @@
       <c r="AC44" s="4"/>
       <c r="AD44" s="4"/>
     </row>
-    <row r="45" spans="1:30" ht="9.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="75" t="s">
+    <row r="45" spans="1:30" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="81"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="M45" s="66" t="s">
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="54"/>
+      <c r="M45" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
-      <c r="Q45" s="66" t="s">
+      <c r="N45" s="54"/>
+      <c r="O45" s="54"/>
+      <c r="Q45" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="R45" s="58"/>
-      <c r="S45" s="58"/>
-      <c r="T45" s="58"/>
-      <c r="U45" s="58"/>
+      <c r="R45" s="54"/>
+      <c r="S45" s="54"/>
+      <c r="T45" s="54"/>
+      <c r="U45" s="54"/>
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
@@ -3986,32 +4012,32 @@
       <c r="AC45" s="4"/>
       <c r="AD45" s="4"/>
     </row>
-    <row r="46" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="64" t="s">
+    <row r="46" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="74" t="s">
+      <c r="B46" s="81"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="61"/>
-      <c r="Q46" s="65" t="s">
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="Q46" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="R46" s="61"/>
-      <c r="S46" s="61"/>
-      <c r="T46" s="61"/>
-      <c r="U46" s="61"/>
+      <c r="R46" s="57"/>
+      <c r="S46" s="57"/>
+      <c r="T46" s="57"/>
+      <c r="U46" s="57"/>
       <c r="V46" s="4"/>
       <c r="W46" s="4" t="s">
         <v>97</v>
@@ -4024,32 +4050,32 @@
       <c r="AC46" s="4"/>
       <c r="AD46" s="4"/>
     </row>
-    <row r="47" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="76" t="s">
+    <row r="47" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="81"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="53"/>
-      <c r="M47" s="52" t="s">
+      <c r="F47" s="81"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="81"/>
+      <c r="K47" s="81"/>
+      <c r="M47" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="N47" s="53"/>
-      <c r="O47" s="53"/>
-      <c r="Q47" s="66" t="s">
+      <c r="N47" s="81"/>
+      <c r="O47" s="81"/>
+      <c r="Q47" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="R47" s="58"/>
-      <c r="S47" s="58"/>
-      <c r="T47" s="58"/>
-      <c r="U47" s="58"/>
+      <c r="R47" s="54"/>
+      <c r="S47" s="54"/>
+      <c r="T47" s="54"/>
+      <c r="U47" s="54"/>
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
@@ -4060,7 +4086,7 @@
       <c r="AC47" s="4"/>
       <c r="AD47" s="4"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -4092,7 +4118,7 @@
       <c r="AC48" s="4"/>
       <c r="AD48" s="4"/>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -4124,7 +4150,7 @@
       <c r="AC49" s="4"/>
       <c r="AD49" s="4"/>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -4156,7 +4182,7 @@
       <c r="AC50" s="4"/>
       <c r="AD50" s="4"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -4188,7 +4214,7 @@
       <c r="AC51" s="4"/>
       <c r="AD51" s="4"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -4222,6 +4248,230 @@
     </row>
   </sheetData>
   <mergeCells count="248">
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="Z21:Z22"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="Z25:Z26"/>
+    <mergeCell ref="Z27:Z28"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="C9:R9"/>
+    <mergeCell ref="R5:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="A44:D45"/>
+    <mergeCell ref="A46:D47"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="Q44:U44"/>
+    <mergeCell ref="Q45:U45"/>
+    <mergeCell ref="Q46:U46"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C12:R12"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="U33:U34"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="A42:D43"/>
+    <mergeCell ref="Y33:Y34"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="W23:W24"/>
+    <mergeCell ref="W25:W26"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="V29:V30"/>
+    <mergeCell ref="W29:W30"/>
+    <mergeCell ref="X29:X30"/>
+    <mergeCell ref="Y29:Y30"/>
+    <mergeCell ref="E46:K46"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="AA23:AA24"/>
+    <mergeCell ref="E45:K45"/>
+    <mergeCell ref="E44:K44"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="S27:S28"/>
+    <mergeCell ref="T27:T28"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="W27:W28"/>
+    <mergeCell ref="X27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="AA27:AA28"/>
+    <mergeCell ref="Y25:Y26"/>
+    <mergeCell ref="E42:K42"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="AA21:AA22"/>
+    <mergeCell ref="AA25:AA26"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="Y35:Y36"/>
+    <mergeCell ref="W33:W34"/>
+    <mergeCell ref="X33:X34"/>
+    <mergeCell ref="E47:K47"/>
+    <mergeCell ref="AB9:AC10"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="Q47:U47"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="AA35:AA36"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="A3:AC3"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="A4:W4"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="U5:W6"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="W21:W22"/>
+    <mergeCell ref="X21:X22"/>
+    <mergeCell ref="Y21:Y22"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="Z29:Z30"/>
+    <mergeCell ref="AB21:AB22"/>
+    <mergeCell ref="AC21:AC22"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="AC25:AC26"/>
+    <mergeCell ref="X23:X24"/>
+    <mergeCell ref="AB23:AB24"/>
+    <mergeCell ref="AC23:AC24"/>
+    <mergeCell ref="E43:K43"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="Q43:U43"/>
+    <mergeCell ref="AB39:AB40"/>
+    <mergeCell ref="AC39:AC40"/>
+    <mergeCell ref="S39:S40"/>
+    <mergeCell ref="T39:T40"/>
+    <mergeCell ref="U39:U40"/>
+    <mergeCell ref="V39:V40"/>
+    <mergeCell ref="W39:W40"/>
+    <mergeCell ref="X39:X40"/>
+    <mergeCell ref="Y39:Y40"/>
+    <mergeCell ref="AA39:AA40"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="Q42:U42"/>
+    <mergeCell ref="Z39:Z40"/>
+    <mergeCell ref="AB37:AB38"/>
+    <mergeCell ref="AC37:AC38"/>
+    <mergeCell ref="AB25:AB26"/>
+    <mergeCell ref="AB35:AB36"/>
+    <mergeCell ref="AA33:AA34"/>
+    <mergeCell ref="AD29:AD30"/>
+    <mergeCell ref="AD31:AD32"/>
+    <mergeCell ref="AD35:AD36"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AB27:AB28"/>
+    <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="AB31:AB32"/>
+    <mergeCell ref="AC31:AC32"/>
+    <mergeCell ref="AA31:AA32"/>
+    <mergeCell ref="AB33:AB34"/>
+    <mergeCell ref="AC33:AC34"/>
+    <mergeCell ref="AC35:AC36"/>
+    <mergeCell ref="AA37:AA38"/>
+    <mergeCell ref="AA29:AA30"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="AD39:AD40"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AD21:AD22"/>
+    <mergeCell ref="AD23:AD24"/>
+    <mergeCell ref="AD25:AD26"/>
+    <mergeCell ref="AD27:AD28"/>
+    <mergeCell ref="AD33:AD34"/>
+    <mergeCell ref="AD37:AD38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="S37:S38"/>
+    <mergeCell ref="T37:T38"/>
+    <mergeCell ref="U37:U38"/>
+    <mergeCell ref="V37:V38"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="S35:S36"/>
+    <mergeCell ref="T35:T36"/>
+    <mergeCell ref="U35:U36"/>
+    <mergeCell ref="V35:V36"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="T33:T34"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
     <mergeCell ref="W37:W38"/>
     <mergeCell ref="X37:X38"/>
     <mergeCell ref="Y37:Y38"/>
@@ -4246,230 +4496,6 @@
     <mergeCell ref="S29:S30"/>
     <mergeCell ref="T29:T30"/>
     <mergeCell ref="U29:U30"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="S37:S38"/>
-    <mergeCell ref="T37:T38"/>
-    <mergeCell ref="U37:U38"/>
-    <mergeCell ref="V37:V38"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="S35:S36"/>
-    <mergeCell ref="T35:T36"/>
-    <mergeCell ref="U35:U36"/>
-    <mergeCell ref="V35:V36"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="T33:T34"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="U25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="AD39:AD40"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AD21:AD22"/>
-    <mergeCell ref="AD23:AD24"/>
-    <mergeCell ref="AD25:AD26"/>
-    <mergeCell ref="AD27:AD28"/>
-    <mergeCell ref="AD33:AD34"/>
-    <mergeCell ref="AD37:AD38"/>
-    <mergeCell ref="AB37:AB38"/>
-    <mergeCell ref="AC37:AC38"/>
-    <mergeCell ref="AB25:AB26"/>
-    <mergeCell ref="AB35:AB36"/>
-    <mergeCell ref="AA33:AA34"/>
-    <mergeCell ref="AD29:AD30"/>
-    <mergeCell ref="AD31:AD32"/>
-    <mergeCell ref="AD35:AD36"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AB27:AB28"/>
-    <mergeCell ref="AC27:AC28"/>
-    <mergeCell ref="AB31:AB32"/>
-    <mergeCell ref="AC31:AC32"/>
-    <mergeCell ref="AA31:AA32"/>
-    <mergeCell ref="AB33:AB34"/>
-    <mergeCell ref="AC33:AC34"/>
-    <mergeCell ref="AC35:AC36"/>
-    <mergeCell ref="AA37:AA38"/>
-    <mergeCell ref="AA29:AA30"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="E43:K43"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="Q43:U43"/>
-    <mergeCell ref="AB39:AB40"/>
-    <mergeCell ref="AC39:AC40"/>
-    <mergeCell ref="S39:S40"/>
-    <mergeCell ref="T39:T40"/>
-    <mergeCell ref="U39:U40"/>
-    <mergeCell ref="V39:V40"/>
-    <mergeCell ref="W39:W40"/>
-    <mergeCell ref="X39:X40"/>
-    <mergeCell ref="Y39:Y40"/>
-    <mergeCell ref="AA39:AA40"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="Q42:U42"/>
-    <mergeCell ref="Z39:Z40"/>
-    <mergeCell ref="Z29:Z30"/>
-    <mergeCell ref="AB21:AB22"/>
-    <mergeCell ref="AC21:AC22"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="AC25:AC26"/>
-    <mergeCell ref="X23:X24"/>
-    <mergeCell ref="AB23:AB24"/>
-    <mergeCell ref="AC23:AC24"/>
-    <mergeCell ref="J8:R8"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="U21:U22"/>
-    <mergeCell ref="V21:V22"/>
-    <mergeCell ref="W21:W22"/>
-    <mergeCell ref="X21:X22"/>
-    <mergeCell ref="Y21:Y22"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="S21:S22"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="Q47:U47"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="AA35:AA36"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="X9:AA9"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="A3:AC3"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="A4:W4"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="U5:W6"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="Y35:Y36"/>
-    <mergeCell ref="W33:W34"/>
-    <mergeCell ref="X33:X34"/>
-    <mergeCell ref="E47:K47"/>
-    <mergeCell ref="AB9:AC10"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="E46:K46"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="AA23:AA24"/>
-    <mergeCell ref="E45:K45"/>
-    <mergeCell ref="E44:K44"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="S27:S28"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="W27:W28"/>
-    <mergeCell ref="X27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="AA27:AA28"/>
-    <mergeCell ref="Y25:Y26"/>
-    <mergeCell ref="E42:K42"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="AA21:AA22"/>
-    <mergeCell ref="AA25:AA26"/>
-    <mergeCell ref="T23:T24"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="V23:V24"/>
-    <mergeCell ref="Y33:Y34"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="W23:W24"/>
-    <mergeCell ref="W25:W26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="V29:V30"/>
-    <mergeCell ref="W29:W30"/>
-    <mergeCell ref="X29:X30"/>
-    <mergeCell ref="Y29:Y30"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="C9:R9"/>
-    <mergeCell ref="R5:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="A44:D45"/>
-    <mergeCell ref="A46:D47"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="Q44:U44"/>
-    <mergeCell ref="Q45:U45"/>
-    <mergeCell ref="Q46:U46"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C12:R12"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="U33:U34"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="A42:D43"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="Z21:Z22"/>
-    <mergeCell ref="Z23:Z24"/>
-    <mergeCell ref="Z25:Z26"/>
-    <mergeCell ref="Z27:Z28"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z7:AA7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.31496062992125978" top="0.74803149606299213" bottom="0.15748031496062989" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="91" orientation="landscape"/>
@@ -4480,285 +4506,285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13:AB38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" customWidth="1"/>
-    <col min="4" max="16" width="6.453125" customWidth="1"/>
-    <col min="17" max="17" width="7.81640625" customWidth="1"/>
-    <col min="18" max="18" width="8.6328125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="16" width="6.5" customWidth="1"/>
+    <col min="17" max="17" width="7.83203125" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" customWidth="1"/>
     <col min="19" max="19" width="5" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="3.453125" customWidth="1"/>
-    <col min="22" max="22" width="5.36328125" customWidth="1"/>
-    <col min="23" max="23" width="5.453125" customWidth="1"/>
-    <col min="24" max="25" width="4.1796875" customWidth="1"/>
+    <col min="21" max="21" width="3.5" customWidth="1"/>
+    <col min="22" max="22" width="5.33203125" customWidth="1"/>
+    <col min="23" max="23" width="5.5" customWidth="1"/>
+    <col min="24" max="25" width="4.1640625" customWidth="1"/>
     <col min="26" max="29" width="6" customWidth="1"/>
-    <col min="30" max="30" width="5.453125" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:40" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2" spans="1:40" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:40" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
-    </row>
-    <row r="3" spans="1:40" s="4" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+    </row>
+    <row r="3" spans="1:40" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-    </row>
-    <row r="4" spans="1:40" s="4" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57"/>
+    </row>
+    <row r="4" spans="1:40" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-    </row>
-    <row r="5" spans="1:40" s="4" customFormat="1" ht="8.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="75"/>
+    </row>
+    <row r="5" spans="1:40" s="4" customFormat="1" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q5" s="8"/>
-      <c r="R5" s="57" t="s">
+      <c r="R5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="58"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="82" t="s">
+      <c r="S5" s="54"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="58"/>
-      <c r="W5" s="59"/>
-      <c r="Z5" s="63" t="s">
+      <c r="V5" s="54"/>
+      <c r="W5" s="71"/>
+      <c r="Z5" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="56"/>
+      <c r="AA5" s="67"/>
+      <c r="AB5" s="67"/>
+      <c r="AC5" s="68"/>
       <c r="AD5" s="28"/>
       <c r="AE5" s="28"/>
       <c r="AF5" s="28"/>
       <c r="AM5" s="28"/>
       <c r="AN5" s="28"/>
     </row>
-    <row r="6" spans="1:40" s="4" customFormat="1" ht="9.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" s="4" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q6" s="8"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="60"/>
-      <c r="V6" s="61"/>
-      <c r="W6" s="62"/>
-      <c r="Z6" s="79" t="s">
+      <c r="R6" s="77"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="78"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="78"/>
+      <c r="Z6" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="79" t="s">
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="AC6" s="59"/>
+      <c r="AC6" s="71"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:40" s="4" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K7" s="83" t="s">
+    <row r="7" spans="1:40" s="4" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="92">
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="97">
         <v>5</v>
       </c>
-      <c r="S7" s="55"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="93">
+      <c r="S7" s="67"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="98">
         <v>44712</v>
       </c>
-      <c r="V7" s="55"/>
-      <c r="W7" s="56"/>
-      <c r="Z7" s="92" t="s">
+      <c r="V7" s="67"/>
+      <c r="W7" s="68"/>
+      <c r="Z7" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="56"/>
-      <c r="AB7" s="92" t="s">
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="56"/>
-    </row>
-    <row r="8" spans="1:40" s="28" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="83" t="s">
+      <c r="AC7" s="68"/>
+    </row>
+    <row r="8" spans="1:40" s="28" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87"/>
-      <c r="R8" s="87"/>
-    </row>
-    <row r="9" spans="1:40" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="94" t="s">
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+    </row>
+    <row r="9" spans="1:40" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="54" t="s">
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="67"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="54" t="s">
+      <c r="T9" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="54" t="s">
+      <c r="U9" s="67"/>
+      <c r="V9" s="67"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="56"/>
-      <c r="AB9" s="54" t="s">
+      <c r="Y9" s="67"/>
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="AC9" s="59"/>
-    </row>
-    <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
+      <c r="AC9" s="71"/>
+    </row>
+    <row r="10" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="32" t="s">
         <v>20</v>
       </c>
@@ -4807,35 +4833,35 @@
       <c r="R10" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="S10" s="48"/>
-      <c r="T10" s="91" t="s">
+      <c r="S10" s="59"/>
+      <c r="T10" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="U10" s="91" t="s">
+      <c r="U10" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="91" t="s">
+      <c r="V10" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="81" t="s">
+      <c r="W10" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="X10" s="81" t="s">
+      <c r="X10" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="Y10" s="81" t="s">
+      <c r="Y10" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="Z10" s="81" t="s">
+      <c r="Z10" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="AA10" s="81" t="s">
+      <c r="AA10" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="62"/>
-    </row>
-    <row r="11" spans="1:40" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB10" s="77"/>
+      <c r="AC10" s="78"/>
+    </row>
+    <row r="11" spans="1:40" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="45"/>
       <c r="B11" s="45"/>
       <c r="C11" s="42" t="s">
@@ -4895,41 +4921,41 @@
       <c r="Y11" s="45"/>
       <c r="Z11" s="45"/>
       <c r="AA11" s="45"/>
-      <c r="AB11" s="81" t="s">
+      <c r="AB11" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="AC11" s="81" t="s">
+      <c r="AC11" s="62" t="s">
         <v>55</v>
       </c>
       <c r="AD11" s="40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="69">
+      <c r="C12" s="87">
         <v>3</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="71"/>
       <c r="S12" s="43">
         <v>4</v>
       </c>
@@ -4967,17 +4993,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67">
+    <row r="13" spans="1:40" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="50">
         <v>1</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="51" t="s">
         <v>109</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="99" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="19" t="s">
@@ -4987,7 +5013,7 @@
         <v>60</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="H13" s="22" t="s">
         <v>62</v>
@@ -5022,11 +5048,11 @@
       <c r="R13" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S13" s="70"/>
-      <c r="T13" s="70"/>
-      <c r="U13" s="70"/>
-      <c r="V13" s="70"/>
-      <c r="W13" s="70"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
       <c r="X13" s="46"/>
       <c r="Y13" s="46"/>
       <c r="Z13" s="46"/>
@@ -5039,7 +5065,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="45"/>
       <c r="B14" s="45"/>
       <c r="C14" s="19" t="s">
@@ -5103,11 +5129,11 @@
       <c r="AC14" s="45"/>
       <c r="AD14" s="45"/>
     </row>
-    <row r="15" spans="1:40" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67">
+    <row r="15" spans="1:40" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="51" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -5158,10 +5184,10 @@
       <c r="R15" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="70"/>
-      <c r="V15" s="70"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
       <c r="W15" s="46"/>
       <c r="X15" s="46"/>
       <c r="Y15" s="46"/>
@@ -5171,11 +5197,11 @@
       <c r="AC15" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="AD15" s="97" t="s">
+      <c r="AD15" s="92" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="45"/>
       <c r="B16" s="45"/>
       <c r="C16" s="22" t="s">
@@ -5237,13 +5263,13 @@
       <c r="AA16" s="35"/>
       <c r="AB16" s="45"/>
       <c r="AC16" s="45"/>
-      <c r="AD16" s="98"/>
-    </row>
-    <row r="17" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="67">
+      <c r="AD16" s="93"/>
+    </row>
+    <row r="17" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="50">
         <v>3</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="51" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="33" t="s">
@@ -5294,10 +5320,10 @@
       <c r="R17" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S17" s="70"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="70"/>
-      <c r="V17" s="70"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="44"/>
       <c r="W17" s="46"/>
       <c r="X17" s="46"/>
       <c r="Y17" s="46"/>
@@ -5311,7 +5337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="19" t="s">
@@ -5375,11 +5401,11 @@
       <c r="AC18" s="45"/>
       <c r="AD18" s="45"/>
     </row>
-    <row r="19" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67">
+    <row r="19" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="50">
         <v>4</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="51" t="s">
         <v>121</v>
       </c>
       <c r="C19" s="33" t="s">
@@ -5430,11 +5456,11 @@
       <c r="R19" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
-      <c r="W19" s="70"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="44"/>
       <c r="X19" s="46"/>
       <c r="Y19" s="46"/>
       <c r="Z19" s="46"/>
@@ -5447,7 +5473,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="45"/>
       <c r="B20" s="45"/>
       <c r="C20" s="20" t="s">
@@ -5511,11 +5537,11 @@
       <c r="AC20" s="45"/>
       <c r="AD20" s="45"/>
     </row>
-    <row r="21" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="67">
+    <row r="21" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="50">
         <v>5</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="51" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="33" t="s">
@@ -5566,11 +5592,11 @@
       <c r="R21" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="70"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
       <c r="X21" s="46"/>
       <c r="Y21" s="46"/>
       <c r="Z21" s="46"/>
@@ -5583,7 +5609,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="45"/>
       <c r="B22" s="45"/>
       <c r="C22" s="20" t="s">
@@ -5647,11 +5673,11 @@
       <c r="AC22" s="45"/>
       <c r="AD22" s="45"/>
     </row>
-    <row r="23" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="67">
+    <row r="23" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="50">
         <v>6</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="51" t="s">
         <v>124</v>
       </c>
       <c r="C23" s="33" t="s">
@@ -5702,10 +5728,10 @@
       <c r="R23" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S23" s="70"/>
-      <c r="T23" s="70"/>
-      <c r="U23" s="70"/>
-      <c r="V23" s="70"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
       <c r="W23" s="46"/>
       <c r="X23" s="46"/>
       <c r="Y23" s="46"/>
@@ -5719,7 +5745,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="45"/>
       <c r="B24" s="45"/>
       <c r="C24" s="19" t="s">
@@ -5783,11 +5809,11 @@
       <c r="AC24" s="45"/>
       <c r="AD24" s="45"/>
     </row>
-    <row r="25" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="67">
+    <row r="25" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="50">
         <v>7</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="51" t="s">
         <v>126</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -5838,11 +5864,11 @@
       <c r="R25" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S25" s="70"/>
-      <c r="T25" s="70"/>
-      <c r="U25" s="70"/>
-      <c r="V25" s="70"/>
-      <c r="W25" s="70"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="44"/>
       <c r="X25" s="46"/>
       <c r="Y25" s="46"/>
       <c r="Z25" s="46"/>
@@ -5855,7 +5881,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="45"/>
       <c r="B26" s="45"/>
       <c r="C26" s="19" t="s">
@@ -5919,11 +5945,11 @@
       <c r="AC26" s="45"/>
       <c r="AD26" s="45"/>
     </row>
-    <row r="27" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="67">
+    <row r="27" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="50">
         <v>8</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="51" t="s">
         <v>127</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -5974,10 +6000,10 @@
       <c r="R27" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S27" s="70"/>
-      <c r="T27" s="70"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="70"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
       <c r="W27" s="46"/>
       <c r="X27" s="46"/>
       <c r="Y27" s="46"/>
@@ -5991,7 +6017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="45"/>
       <c r="B28" s="45"/>
       <c r="C28" s="19" t="s">
@@ -6055,11 +6081,11 @@
       <c r="AC28" s="45"/>
       <c r="AD28" s="45"/>
     </row>
-    <row r="29" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="67">
+    <row r="29" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="50">
         <v>9</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="51" t="s">
         <v>129</v>
       </c>
       <c r="C29" s="19" t="s">
@@ -6110,13 +6136,13 @@
       <c r="R29" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S29" s="90"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="90"/>
-      <c r="V29" s="90"/>
-      <c r="W29" s="90"/>
-      <c r="X29" s="89"/>
-      <c r="Y29" s="89"/>
+      <c r="S29" s="47"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="47"/>
+      <c r="V29" s="47"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="49"/>
+      <c r="Y29" s="49"/>
       <c r="Z29" s="46"/>
       <c r="AA29" s="46"/>
       <c r="AB29" s="46"/>
@@ -6127,7 +6153,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="45"/>
       <c r="B30" s="45"/>
       <c r="C30" s="19" t="s">
@@ -6191,11 +6217,11 @@
       <c r="AC30" s="45"/>
       <c r="AD30" s="45"/>
     </row>
-    <row r="31" spans="1:30" s="15" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="72">
+    <row r="31" spans="1:30" s="15" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="83">
         <v>10</v>
       </c>
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="51" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -6246,10 +6272,10 @@
       <c r="R31" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S31" s="70"/>
-      <c r="T31" s="70"/>
-      <c r="U31" s="70"/>
-      <c r="V31" s="70"/>
+      <c r="S31" s="44"/>
+      <c r="T31" s="44"/>
+      <c r="U31" s="44"/>
+      <c r="V31" s="44"/>
       <c r="W31" s="46"/>
       <c r="X31" s="46"/>
       <c r="Y31" s="46"/>
@@ -6263,7 +6289,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="15" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" s="15" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="45"/>
       <c r="B32" s="45"/>
       <c r="C32" s="19" t="s">
@@ -6327,11 +6353,11 @@
       <c r="AC32" s="45"/>
       <c r="AD32" s="45"/>
     </row>
-    <row r="33" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67">
+    <row r="33" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="50">
         <v>11</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="51" t="s">
         <v>133</v>
       </c>
       <c r="C33" s="19" t="s">
@@ -6382,10 +6408,10 @@
       <c r="R33" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S33" s="70"/>
-      <c r="T33" s="70"/>
-      <c r="U33" s="70"/>
-      <c r="V33" s="70"/>
+      <c r="S33" s="44"/>
+      <c r="T33" s="44"/>
+      <c r="U33" s="44"/>
+      <c r="V33" s="44"/>
       <c r="W33" s="46"/>
       <c r="X33" s="46"/>
       <c r="Y33" s="46"/>
@@ -6399,7 +6425,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="45"/>
       <c r="B34" s="45"/>
       <c r="C34" s="22" t="s">
@@ -6451,11 +6477,11 @@
       <c r="AC34" s="45"/>
       <c r="AD34" s="45"/>
     </row>
-    <row r="35" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="67">
+    <row r="35" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="50">
         <v>12</v>
       </c>
-      <c r="B35" s="95" t="s">
+      <c r="B35" s="94" t="s">
         <v>134</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -6506,11 +6532,11 @@
       <c r="R35" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S35" s="70"/>
+      <c r="S35" s="44"/>
       <c r="T35" s="46"/>
-      <c r="U35" s="70"/>
-      <c r="V35" s="70"/>
-      <c r="W35" s="70"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="44"/>
       <c r="X35" s="46"/>
       <c r="Y35" s="46"/>
       <c r="Z35" s="46"/>
@@ -6519,9 +6545,9 @@
       <c r="AC35" s="46"/>
       <c r="AD35" s="46"/>
     </row>
-    <row r="36" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="45"/>
-      <c r="B36" s="60"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="19" t="s">
         <v>66</v>
       </c>
@@ -6583,11 +6609,11 @@
       <c r="AC36" s="45"/>
       <c r="AD36" s="45"/>
     </row>
-    <row r="37" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="67">
+    <row r="37" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="50">
         <v>13</v>
       </c>
-      <c r="B37" s="95" t="s">
+      <c r="B37" s="94" t="s">
         <v>136</v>
       </c>
       <c r="C37" s="19" t="s">
@@ -6638,11 +6664,11 @@
       <c r="R37" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S37" s="70"/>
+      <c r="S37" s="44"/>
       <c r="T37" s="46"/>
-      <c r="U37" s="70"/>
-      <c r="V37" s="70"/>
-      <c r="W37" s="70"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="44"/>
       <c r="X37" s="46"/>
       <c r="Y37" s="46"/>
       <c r="Z37" s="46"/>
@@ -6651,9 +6677,9 @@
       <c r="AC37" s="46"/>
       <c r="AD37" s="46"/>
     </row>
-    <row r="38" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="45"/>
-      <c r="B38" s="60"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="19" t="s">
         <v>135</v>
       </c>
@@ -6715,11 +6741,11 @@
       <c r="AC38" s="45"/>
       <c r="AD38" s="45"/>
     </row>
-    <row r="39" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="67">
+    <row r="39" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="50">
         <v>14</v>
       </c>
-      <c r="B39" s="96" t="s">
+      <c r="B39" s="91" t="s">
         <v>137</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -6770,15 +6796,15 @@
       <c r="R39" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S39" s="70">
+      <c r="S39" s="44">
         <v>18</v>
       </c>
       <c r="T39" s="46">
         <v>144</v>
       </c>
-      <c r="U39" s="70"/>
-      <c r="V39" s="70"/>
-      <c r="W39" s="70"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="44"/>
       <c r="X39" s="46">
         <v>13</v>
       </c>
@@ -6789,9 +6815,9 @@
       <c r="AC39" s="46"/>
       <c r="AD39" s="46"/>
     </row>
-    <row r="40" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="45"/>
-      <c r="B40" s="60"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="19" t="s">
         <v>25</v>
       </c>
@@ -6853,11 +6879,11 @@
       <c r="AC40" s="45"/>
       <c r="AD40" s="45"/>
     </row>
-    <row r="41" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="67">
+    <row r="41" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="50">
         <v>15</v>
       </c>
-      <c r="B41" s="96" t="s">
+      <c r="B41" s="91" t="s">
         <v>138</v>
       </c>
       <c r="C41" s="19" t="s">
@@ -6908,15 +6934,15 @@
       <c r="R41" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S41" s="70">
+      <c r="S41" s="44">
         <v>17</v>
       </c>
       <c r="T41" s="46">
         <v>136</v>
       </c>
-      <c r="U41" s="70"/>
-      <c r="V41" s="70"/>
-      <c r="W41" s="70"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
       <c r="X41" s="46">
         <v>13</v>
       </c>
@@ -6929,9 +6955,9 @@
       <c r="AC41" s="46"/>
       <c r="AD41" s="46"/>
     </row>
-    <row r="42" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="45"/>
-      <c r="B42" s="60"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="19" t="s">
         <v>25</v>
       </c>
@@ -6993,11 +7019,11 @@
       <c r="AC42" s="45"/>
       <c r="AD42" s="45"/>
     </row>
-    <row r="43" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="67">
+    <row r="43" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="50">
         <v>16</v>
       </c>
-      <c r="B43" s="96" t="s">
+      <c r="B43" s="91" t="s">
         <v>140</v>
       </c>
       <c r="C43" s="19" t="s">
@@ -7048,15 +7074,15 @@
       <c r="R43" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="S43" s="70">
+      <c r="S43" s="44">
         <v>18</v>
       </c>
       <c r="T43" s="46">
         <v>144</v>
       </c>
-      <c r="U43" s="70"/>
-      <c r="V43" s="70"/>
-      <c r="W43" s="70"/>
+      <c r="U43" s="44"/>
+      <c r="V43" s="44"/>
+      <c r="W43" s="44"/>
       <c r="X43" s="46">
         <v>13</v>
       </c>
@@ -7067,9 +7093,9 @@
       <c r="AC43" s="46"/>
       <c r="AD43" s="46"/>
     </row>
-    <row r="44" spans="1:30" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="45"/>
-      <c r="B44" s="60"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="19" t="s">
         <v>25</v>
       </c>
@@ -7131,7 +7157,7 @@
       <c r="AC44" s="45"/>
       <c r="AD44" s="45"/>
     </row>
-    <row r="45" spans="1:30" ht="5.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" ht="5.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
@@ -7163,32 +7189,32 @@
       <c r="AC45" s="12"/>
       <c r="AD45" s="12"/>
     </row>
-    <row r="46" spans="1:30" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="64" t="s">
+    <row r="46" spans="1:30" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="74" t="s">
+      <c r="B46" s="81"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="61"/>
-      <c r="Q46" s="65" t="s">
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+      <c r="Q46" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="R46" s="61"/>
-      <c r="S46" s="61"/>
-      <c r="T46" s="61"/>
-      <c r="U46" s="61"/>
+      <c r="R46" s="57"/>
+      <c r="S46" s="57"/>
+      <c r="T46" s="57"/>
+      <c r="U46" s="57"/>
       <c r="V46" s="4"/>
       <c r="W46" s="4" t="s">
         <v>97</v>
@@ -7201,32 +7227,32 @@
       <c r="AC46" s="12"/>
       <c r="AD46" s="12"/>
     </row>
-    <row r="47" spans="1:30" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="75" t="s">
+    <row r="47" spans="1:30" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="81"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="M47" s="66" t="s">
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="54"/>
+      <c r="M47" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
-      <c r="Q47" s="66" t="s">
+      <c r="N47" s="54"/>
+      <c r="O47" s="54"/>
+      <c r="Q47" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="R47" s="58"/>
-      <c r="S47" s="58"/>
-      <c r="T47" s="58"/>
-      <c r="U47" s="58"/>
+      <c r="R47" s="54"/>
+      <c r="S47" s="54"/>
+      <c r="T47" s="54"/>
+      <c r="U47" s="54"/>
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
@@ -7237,32 +7263,32 @@
       <c r="AC47" s="12"/>
       <c r="AD47" s="12"/>
     </row>
-    <row r="48" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="64" t="s">
+    <row r="48" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="74" t="s">
+      <c r="B48" s="81"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="M48" s="65"/>
-      <c r="N48" s="61"/>
-      <c r="O48" s="61"/>
-      <c r="Q48" s="65" t="s">
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="57"/>
+      <c r="Q48" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="R48" s="61"/>
-      <c r="S48" s="61"/>
-      <c r="T48" s="61"/>
-      <c r="U48" s="61"/>
+      <c r="R48" s="57"/>
+      <c r="S48" s="57"/>
+      <c r="T48" s="57"/>
+      <c r="U48" s="57"/>
       <c r="V48" s="4"/>
       <c r="W48" s="4" t="s">
         <v>97</v>
@@ -7275,32 +7301,32 @@
       <c r="AC48" s="4"/>
       <c r="AD48" s="4"/>
     </row>
-    <row r="49" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="75" t="s">
+    <row r="49" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="81"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="M49" s="66" t="s">
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="54"/>
+      <c r="M49" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="N49" s="58"/>
-      <c r="O49" s="58"/>
-      <c r="Q49" s="66" t="s">
+      <c r="N49" s="54"/>
+      <c r="O49" s="54"/>
+      <c r="Q49" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="R49" s="58"/>
-      <c r="S49" s="58"/>
-      <c r="T49" s="58"/>
-      <c r="U49" s="58"/>
+      <c r="R49" s="54"/>
+      <c r="S49" s="54"/>
+      <c r="T49" s="54"/>
+      <c r="U49" s="54"/>
       <c r="V49" s="4"/>
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
@@ -7311,32 +7337,32 @@
       <c r="AC49" s="4"/>
       <c r="AD49" s="4"/>
     </row>
-    <row r="50" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="64" t="s">
+    <row r="50" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="74" t="s">
+      <c r="B50" s="81"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61"/>
-      <c r="M50" s="65"/>
-      <c r="N50" s="61"/>
-      <c r="O50" s="61"/>
-      <c r="Q50" s="65" t="s">
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="57"/>
+      <c r="Q50" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="R50" s="61"/>
-      <c r="S50" s="61"/>
-      <c r="T50" s="61"/>
-      <c r="U50" s="61"/>
+      <c r="R50" s="57"/>
+      <c r="S50" s="57"/>
+      <c r="T50" s="57"/>
+      <c r="U50" s="57"/>
       <c r="V50" s="4"/>
       <c r="W50" s="4" t="s">
         <v>97</v>
@@ -7349,32 +7375,32 @@
       <c r="AC50" s="4"/>
       <c r="AD50" s="4"/>
     </row>
-    <row r="51" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="53"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="76" t="s">
+    <row r="51" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="81"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="53"/>
-      <c r="M51" s="52" t="s">
+      <c r="F51" s="81"/>
+      <c r="G51" s="81"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="81"/>
+      <c r="K51" s="81"/>
+      <c r="M51" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="N51" s="53"/>
-      <c r="O51" s="53"/>
-      <c r="Q51" s="66" t="s">
+      <c r="N51" s="81"/>
+      <c r="O51" s="81"/>
+      <c r="Q51" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="R51" s="58"/>
-      <c r="S51" s="58"/>
-      <c r="T51" s="58"/>
-      <c r="U51" s="58"/>
+      <c r="R51" s="54"/>
+      <c r="S51" s="54"/>
+      <c r="T51" s="54"/>
+      <c r="U51" s="54"/>
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
       <c r="X51" s="4"/>
@@ -7385,7 +7411,7 @@
       <c r="AC51" s="4"/>
       <c r="AD51" s="4"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -7417,7 +7443,7 @@
       <c r="AC52" s="4"/>
       <c r="AD52" s="4"/>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -7449,7 +7475,7 @@
       <c r="AC53" s="4"/>
       <c r="AD53" s="4"/>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -7481,7 +7507,7 @@
       <c r="AC54" s="4"/>
       <c r="AD54" s="4"/>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -7513,7 +7539,7 @@
       <c r="AC55" s="4"/>
       <c r="AD55" s="4"/>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -7547,6 +7573,257 @@
     </row>
   </sheetData>
   <mergeCells count="275">
+    <mergeCell ref="AA41:AA42"/>
+    <mergeCell ref="AA43:AA44"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AA21:AA22"/>
+    <mergeCell ref="AA25:AA26"/>
+    <mergeCell ref="AA27:AA28"/>
+    <mergeCell ref="AA29:AA30"/>
+    <mergeCell ref="AA31:AA32"/>
+    <mergeCell ref="AA33:AA34"/>
+    <mergeCell ref="AA39:AA40"/>
+    <mergeCell ref="AA23:AA24"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="J8:R8"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="A3:AC3"/>
+    <mergeCell ref="A4:W4"/>
+    <mergeCell ref="R5:T6"/>
+    <mergeCell ref="U5:W6"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="AC11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="AB13:AB14"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="X13:X14"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AB11"/>
+    <mergeCell ref="AB9:AC10"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="C12:R12"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:R9"/>
+    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="AB15:AB16"/>
+    <mergeCell ref="AC15:AC16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="W15:W16"/>
+    <mergeCell ref="X15:X16"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="X19:X20"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="W17:W18"/>
+    <mergeCell ref="X17:X18"/>
+    <mergeCell ref="Y17:Y18"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="AB17:AB18"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="AB23:AB24"/>
+    <mergeCell ref="AC23:AC24"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="W23:W24"/>
+    <mergeCell ref="X23:X24"/>
+    <mergeCell ref="X21:X22"/>
+    <mergeCell ref="Y21:Y22"/>
+    <mergeCell ref="Z21:Z22"/>
+    <mergeCell ref="AB21:AB22"/>
+    <mergeCell ref="AC21:AC22"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="W21:W22"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="X25:X26"/>
+    <mergeCell ref="Y25:Y26"/>
+    <mergeCell ref="Z25:Z26"/>
+    <mergeCell ref="AB25:AB26"/>
+    <mergeCell ref="AC25:AC26"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="W25:W26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="Z27:Z28"/>
+    <mergeCell ref="AB27:AB28"/>
+    <mergeCell ref="AC27:AC28"/>
+    <mergeCell ref="S27:S28"/>
+    <mergeCell ref="T27:T28"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="W27:W28"/>
+    <mergeCell ref="X27:X28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="Y29:Y30"/>
+    <mergeCell ref="Z29:Z30"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="S29:S30"/>
+    <mergeCell ref="T29:T30"/>
+    <mergeCell ref="U29:U30"/>
+    <mergeCell ref="V29:V30"/>
+    <mergeCell ref="W29:W30"/>
+    <mergeCell ref="X29:X30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="X31:X32"/>
+    <mergeCell ref="Y31:Y32"/>
+    <mergeCell ref="Z31:Z32"/>
+    <mergeCell ref="AB31:AB32"/>
+    <mergeCell ref="AC31:AC32"/>
+    <mergeCell ref="S31:S32"/>
+    <mergeCell ref="T31:T32"/>
+    <mergeCell ref="U31:U32"/>
+    <mergeCell ref="V31:V32"/>
+    <mergeCell ref="W31:W32"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="Y35:Y36"/>
+    <mergeCell ref="Z35:Z36"/>
+    <mergeCell ref="AB35:AB36"/>
+    <mergeCell ref="AC35:AC36"/>
+    <mergeCell ref="S35:S36"/>
+    <mergeCell ref="T35:T36"/>
+    <mergeCell ref="U35:U36"/>
+    <mergeCell ref="V35:V36"/>
+    <mergeCell ref="W35:W36"/>
+    <mergeCell ref="X35:X36"/>
+    <mergeCell ref="AB33:AB34"/>
+    <mergeCell ref="AC33:AC34"/>
+    <mergeCell ref="S33:S34"/>
+    <mergeCell ref="T33:T34"/>
+    <mergeCell ref="U33:U34"/>
+    <mergeCell ref="V33:V34"/>
+    <mergeCell ref="W33:W34"/>
+    <mergeCell ref="X33:X34"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="X37:X38"/>
+    <mergeCell ref="Y37:Y38"/>
+    <mergeCell ref="Z37:Z38"/>
+    <mergeCell ref="AB37:AB38"/>
+    <mergeCell ref="AC37:AC38"/>
+    <mergeCell ref="S37:S38"/>
+    <mergeCell ref="T37:T38"/>
+    <mergeCell ref="U37:U38"/>
+    <mergeCell ref="V37:V38"/>
+    <mergeCell ref="W37:W38"/>
+    <mergeCell ref="W41:W42"/>
+    <mergeCell ref="X41:X42"/>
+    <mergeCell ref="A46:D47"/>
+    <mergeCell ref="E46:K46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="Q46:U46"/>
+    <mergeCell ref="E47:K47"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="S43:S44"/>
+    <mergeCell ref="T43:T44"/>
+    <mergeCell ref="U43:U44"/>
+    <mergeCell ref="V43:V44"/>
+    <mergeCell ref="W43:W44"/>
+    <mergeCell ref="X43:X44"/>
+    <mergeCell ref="A50:D51"/>
+    <mergeCell ref="E50:K50"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="Q50:U50"/>
+    <mergeCell ref="E51:K51"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="Q47:U47"/>
+    <mergeCell ref="A48:D49"/>
+    <mergeCell ref="E48:K48"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="Q48:U48"/>
+    <mergeCell ref="E49:K49"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="Q49:U49"/>
+    <mergeCell ref="AD31:AD32"/>
+    <mergeCell ref="AD33:AD34"/>
+    <mergeCell ref="AD35:AD36"/>
+    <mergeCell ref="AD37:AD38"/>
+    <mergeCell ref="Y33:Y34"/>
+    <mergeCell ref="Z33:Z34"/>
+    <mergeCell ref="AD43:AD44"/>
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AD15:AD16"/>
+    <mergeCell ref="AD17:AD18"/>
+    <mergeCell ref="AD19:AD20"/>
+    <mergeCell ref="AD21:AD22"/>
+    <mergeCell ref="AD23:AD24"/>
+    <mergeCell ref="AD25:AD26"/>
+    <mergeCell ref="AD27:AD28"/>
+    <mergeCell ref="AD29:AD30"/>
+    <mergeCell ref="Y43:Y44"/>
+    <mergeCell ref="Z43:Z44"/>
+    <mergeCell ref="AB43:AB44"/>
+    <mergeCell ref="AC43:AC44"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AC17:AC18"/>
+    <mergeCell ref="Y19:Y20"/>
+    <mergeCell ref="Z19:Z20"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="AB39:AB40"/>
     <mergeCell ref="AC39:AC40"/>
@@ -7571,260 +7848,9 @@
     <mergeCell ref="T41:T42"/>
     <mergeCell ref="U41:U42"/>
     <mergeCell ref="V41:V42"/>
-    <mergeCell ref="AD31:AD32"/>
-    <mergeCell ref="AD33:AD34"/>
-    <mergeCell ref="AD35:AD36"/>
-    <mergeCell ref="AD37:AD38"/>
-    <mergeCell ref="Y33:Y34"/>
-    <mergeCell ref="Z33:Z34"/>
-    <mergeCell ref="AD43:AD44"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AD15:AD16"/>
-    <mergeCell ref="AD17:AD18"/>
-    <mergeCell ref="AD19:AD20"/>
-    <mergeCell ref="AD21:AD22"/>
-    <mergeCell ref="AD23:AD24"/>
-    <mergeCell ref="AD25:AD26"/>
-    <mergeCell ref="AD27:AD28"/>
-    <mergeCell ref="AD29:AD30"/>
-    <mergeCell ref="Y43:Y44"/>
-    <mergeCell ref="Z43:Z44"/>
-    <mergeCell ref="AB43:AB44"/>
-    <mergeCell ref="AC43:AC44"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AC17:AC18"/>
-    <mergeCell ref="Y19:Y20"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="A50:D51"/>
-    <mergeCell ref="E50:K50"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="Q50:U50"/>
-    <mergeCell ref="E51:K51"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="Q47:U47"/>
-    <mergeCell ref="A48:D49"/>
-    <mergeCell ref="E48:K48"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="Q48:U48"/>
-    <mergeCell ref="E49:K49"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="Q49:U49"/>
-    <mergeCell ref="W41:W42"/>
-    <mergeCell ref="X41:X42"/>
-    <mergeCell ref="A46:D47"/>
-    <mergeCell ref="E46:K46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="Q46:U46"/>
-    <mergeCell ref="E47:K47"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="S43:S44"/>
-    <mergeCell ref="T43:T44"/>
-    <mergeCell ref="U43:U44"/>
-    <mergeCell ref="V43:V44"/>
-    <mergeCell ref="W43:W44"/>
-    <mergeCell ref="X43:X44"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="X37:X38"/>
-    <mergeCell ref="Y37:Y38"/>
-    <mergeCell ref="Z37:Z38"/>
-    <mergeCell ref="AB37:AB38"/>
-    <mergeCell ref="AC37:AC38"/>
-    <mergeCell ref="S37:S38"/>
-    <mergeCell ref="T37:T38"/>
-    <mergeCell ref="U37:U38"/>
-    <mergeCell ref="V37:V38"/>
-    <mergeCell ref="W37:W38"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="Y35:Y36"/>
-    <mergeCell ref="Z35:Z36"/>
-    <mergeCell ref="AB35:AB36"/>
-    <mergeCell ref="AC35:AC36"/>
-    <mergeCell ref="S35:S36"/>
-    <mergeCell ref="T35:T36"/>
-    <mergeCell ref="U35:U36"/>
-    <mergeCell ref="V35:V36"/>
-    <mergeCell ref="W35:W36"/>
-    <mergeCell ref="X35:X36"/>
-    <mergeCell ref="AB33:AB34"/>
-    <mergeCell ref="AC33:AC34"/>
-    <mergeCell ref="S33:S34"/>
-    <mergeCell ref="T33:T34"/>
-    <mergeCell ref="U33:U34"/>
-    <mergeCell ref="V33:V34"/>
-    <mergeCell ref="W33:W34"/>
-    <mergeCell ref="X33:X34"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="X31:X32"/>
-    <mergeCell ref="Y31:Y32"/>
-    <mergeCell ref="Z31:Z32"/>
-    <mergeCell ref="AB31:AB32"/>
-    <mergeCell ref="AC31:AC32"/>
-    <mergeCell ref="S31:S32"/>
-    <mergeCell ref="T31:T32"/>
-    <mergeCell ref="U31:U32"/>
-    <mergeCell ref="V31:V32"/>
-    <mergeCell ref="W31:W32"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="Y29:Y30"/>
-    <mergeCell ref="Z29:Z30"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="S29:S30"/>
-    <mergeCell ref="T29:T30"/>
-    <mergeCell ref="U29:U30"/>
-    <mergeCell ref="V29:V30"/>
-    <mergeCell ref="W29:W30"/>
-    <mergeCell ref="X29:X30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="Z27:Z28"/>
-    <mergeCell ref="AB27:AB28"/>
-    <mergeCell ref="AC27:AC28"/>
-    <mergeCell ref="S27:S28"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="W27:W28"/>
-    <mergeCell ref="X27:X28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="X25:X26"/>
-    <mergeCell ref="Y25:Y26"/>
-    <mergeCell ref="Z25:Z26"/>
-    <mergeCell ref="AB25:AB26"/>
-    <mergeCell ref="AC25:AC26"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="U25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="W25:W26"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="Z23:Z24"/>
-    <mergeCell ref="AB23:AB24"/>
-    <mergeCell ref="AC23:AC24"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="T23:T24"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="V23:V24"/>
-    <mergeCell ref="W23:W24"/>
-    <mergeCell ref="X23:X24"/>
-    <mergeCell ref="X21:X22"/>
-    <mergeCell ref="Y21:Y22"/>
-    <mergeCell ref="Z21:Z22"/>
-    <mergeCell ref="AB21:AB22"/>
-    <mergeCell ref="AC21:AC22"/>
-    <mergeCell ref="S21:S22"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="U21:U22"/>
-    <mergeCell ref="V21:V22"/>
-    <mergeCell ref="W21:W22"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="X19:X20"/>
-    <mergeCell ref="S17:S18"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:V18"/>
-    <mergeCell ref="W17:W18"/>
-    <mergeCell ref="X17:X18"/>
-    <mergeCell ref="Y17:Y18"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="AB17:AB18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="Y15:Y16"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="AB15:AB16"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="V15:V16"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="AC11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Z10:Z11"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="X13:X14"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AB11"/>
-    <mergeCell ref="AB9:AC10"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="C12:R12"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:R9"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="A3:AC3"/>
-    <mergeCell ref="A4:W4"/>
-    <mergeCell ref="R5:T6"/>
-    <mergeCell ref="U5:W6"/>
-    <mergeCell ref="Z5:AC5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="J8:R8"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="X9:AA9"/>
-    <mergeCell ref="AA41:AA42"/>
-    <mergeCell ref="AA43:AA44"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AA21:AA22"/>
-    <mergeCell ref="AA25:AA26"/>
-    <mergeCell ref="AA27:AA28"/>
-    <mergeCell ref="AA29:AA30"/>
-    <mergeCell ref="AA31:AA32"/>
-    <mergeCell ref="AA33:AA34"/>
-    <mergeCell ref="AA39:AA40"/>
-    <mergeCell ref="AA23:AA24"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.11811023622047249" top="0.35433070866141742" bottom="0.19685039370078741" header="0.31496062992125978" footer="0.11811023622047249"/>
-  <pageSetup paperSize="9" scale="91" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="91" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7836,12 +7862,12 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="132.453125" customWidth="1"/>
+    <col min="1" max="1" width="132.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>141</v>
       </c>
@@ -7849,7 +7875,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>143</v>
       </c>
@@ -7857,7 +7883,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>144</v>
       </c>
@@ -7865,7 +7891,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>146</v>
       </c>
@@ -7873,7 +7899,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>147</v>
       </c>
@@ -7881,7 +7907,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>149</v>
       </c>
@@ -7889,7 +7915,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>151</v>
       </c>
@@ -7897,7 +7923,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>152</v>
       </c>
@@ -7905,7 +7931,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>154</v>
       </c>
@@ -7913,7 +7939,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>156</v>
       </c>
@@ -7921,7 +7947,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>158</v>
       </c>
@@ -7929,7 +7955,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>160</v>
       </c>
@@ -7937,7 +7963,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>162</v>
       </c>
@@ -7945,7 +7971,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>163</v>
       </c>
@@ -7953,7 +7979,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>165</v>
       </c>
@@ -7961,7 +7987,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>167</v>
       </c>

</xml_diff>